<commit_message>
Update data processing section and add uncertainty propagation details in the report. Replace references to processed and raw data subsections with new structure, including example calculations and a summary of uncertainties by tool. Update related files and remove obsolete .blg file.
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wrca-my.sharepoint.com/personal/huj26_mywrca_ca/Documents/12/Chemistry HL/Chemistry IA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1599" documentId="8_{ED69E5BD-9A97-5849-9651-1A764BC4410F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DEF5CEB-B0D6-E742-95C3-B812919AFE8C}"/>
+  <xr:revisionPtr revIDLastSave="1772" documentId="8_{ED69E5BD-9A97-5849-9651-1A764BC4410F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC7D8A26-372A-B54C-AB12-C1D4ADB4920F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{3196E468-6A35-EA40-9409-42F714E37880}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="56">
   <si>
     <t>Target (°C)</t>
   </si>
@@ -240,6 +240,12 @@
   </si>
   <si>
     <t>Average Initial Rate (kPa/s)</t>
+  </si>
+  <si>
+    <t>Uncertainty in Avg Rate (kPa/s)</t>
+  </si>
+  <si>
+    <t>Initial Rate SD (kPa/s)</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1586,6 +1592,15 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1809,6 +1824,91 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Processed Data'!$O$3:$O$42</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="40"/>
+                  <c:pt idx="0">
+                    <c:v>4.336020064529226E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.9758788168523553E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.0545694411494834E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.9442640509971881E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1.3418992883223374E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>1.847383338671214E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>6.8257707623388592E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>4.6718455346896962E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Processed Data'!$O$3:$O$42</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="40"/>
+                  <c:pt idx="0">
+                    <c:v>4.336020064529226E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.9758788168523553E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.0545694411494834E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.9442640509971881E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1.3418992883223374E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>1.847383338671214E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>6.8257707623388592E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>4.6718455346896962E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Processed Data'!$C$3:$C$42</c:f>
@@ -1846,31 +1946,31 @@
             <c:numRef>
               <c:f>'Processed Data'!$O$3:$O$42</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="40"/>
-                <c:pt idx="0" formatCode="0.00000">
-                  <c:v>0</c:v>
+                <c:pt idx="0">
+                  <c:v>4.336020064529226E-3</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00000">
-                  <c:v>0</c:v>
+                <c:pt idx="5">
+                  <c:v>4.9758788168523553E-3</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="0.00000">
-                  <c:v>0</c:v>
+                <c:pt idx="10">
+                  <c:v>7.0545694411494834E-3</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="0.00000">
-                  <c:v>0</c:v>
+                <c:pt idx="15">
+                  <c:v>1.9442640509971881E-2</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="0.00000">
-                  <c:v>0</c:v>
+                <c:pt idx="20">
+                  <c:v>1.3418992883223374E-2</c:v>
                 </c:pt>
-                <c:pt idx="25" formatCode="0.00000">
-                  <c:v>0</c:v>
+                <c:pt idx="25">
+                  <c:v>1.847383338671214E-2</c:v>
                 </c:pt>
-                <c:pt idx="30" formatCode="0.00000">
-                  <c:v>0</c:v>
+                <c:pt idx="30">
+                  <c:v>6.8257707623388592E-2</c:v>
                 </c:pt>
-                <c:pt idx="35" formatCode="0.00000">
-                  <c:v>0</c:v>
+                <c:pt idx="35">
+                  <c:v>4.6718455346896962E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2060,6 +2160,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="8.0927595927876312E-3"/>
+              <c:y val="0.37841081275123239"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2742,16 +2850,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1022684</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>44561</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>8912</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>155964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>256228</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>57039</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>534736</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2777,10 +2885,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3103,7 +3207,7 @@
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="I3" sqref="I3:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4689,8 +4793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDC91D6-17D9-9B43-8128-D1F89723CF23}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4700,15 +4804,16 @@
     <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="15.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" style="114" customWidth="1"/>
-    <col min="15" max="15" width="27" style="102" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30" style="114" customWidth="1"/>
+    <col min="15" max="15" width="25.5" style="102" customWidth="1"/>
     <col min="16" max="16" width="10.83203125" style="1"/>
     <col min="17" max="17" width="28" style="1" customWidth="1"/>
     <col min="18" max="18" width="9.6640625" style="1" customWidth="1"/>
@@ -4726,15 +4831,15 @@
       <c r="C1" s="147"/>
       <c r="D1" s="147"/>
       <c r="E1" s="147"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
       <c r="J1" s="147"/>
       <c r="K1" s="147"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
       <c r="O1" s="148"/>
       <c r="Q1" s="105"/>
       <c r="R1" s="105"/>
@@ -4757,35 +4862,35 @@
       <c r="E2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="110" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="110" t="s">
+      <c r="F2" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="109" t="s">
+      <c r="H2" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="115" t="s">
+      <c r="I2" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="110" t="s">
+      <c r="K2" s="110" t="s">
         <v>51</v>
       </c>
+      <c r="L2" s="121" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="96" t="s">
+        <v>53</v>
+      </c>
       <c r="N2" s="121" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="96" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="O2" s="121" t="s">
+        <v>55</v>
       </c>
       <c r="Q2" s="104"/>
       <c r="R2" s="104"/>
@@ -4793,52 +4898,57 @@
       <c r="T2" s="104"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="161">
+      <c r="A3" s="164">
         <v>1</v>
       </c>
       <c r="B3" s="122">
         <v>1</v>
       </c>
-      <c r="C3" s="162">
+      <c r="C3" s="165">
         <v>15</v>
       </c>
-      <c r="D3" s="162">
+      <c r="D3" s="165">
         <f>C3+273.15</f>
         <v>288.14999999999998</v>
       </c>
       <c r="E3" s="123">
         <v>4</v>
       </c>
-      <c r="F3" s="124">
-        <v>14.4</v>
-      </c>
-      <c r="G3" s="125">
-        <v>15.1</v>
-      </c>
-      <c r="H3" s="125">
-        <f>AVERAGE(F3:G3)</f>
+      <c r="F3" s="26">
         <v>14.75</v>
       </c>
-      <c r="I3" s="126">
-        <f>H3+274.15</f>
+      <c r="G3" s="126">
+        <f>F3+274.15</f>
         <v>288.89999999999998</v>
       </c>
-      <c r="J3" s="127">
+      <c r="H3" s="127">
         <v>25</v>
       </c>
-      <c r="K3" s="128">
+      <c r="I3" s="128">
         <v>0.3</v>
       </c>
-      <c r="L3" s="124">
+      <c r="J3" s="124">
         <v>26.6</v>
       </c>
-      <c r="M3" s="125"/>
-      <c r="N3" s="129"/>
-      <c r="O3" s="158" t="e">
-        <f>AVERAGE(N3:N7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S3" s="164"/>
+      <c r="K3" s="125">
+        <v>41.6</v>
+      </c>
+      <c r="L3" s="129">
+        <v>5.94E-3</v>
+      </c>
+      <c r="M3" s="158">
+        <f>AVERAGE(L3:L7)</f>
+        <v>1.0232E-2</v>
+      </c>
+      <c r="N3" s="161">
+        <f>O3/SQRT(5)</f>
+        <v>1.9391271232180748E-3</v>
+      </c>
+      <c r="O3" s="161">
+        <f>_xlfn.STDEV.S(L3:L7)</f>
+        <v>4.336020064529226E-3</v>
+      </c>
+      <c r="S3" s="167"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="137"/>
@@ -4850,33 +4960,32 @@
       <c r="E4" s="111">
         <v>5</v>
       </c>
-      <c r="F4" s="27">
-        <v>15.4</v>
-      </c>
-      <c r="G4" s="17">
-        <v>16</v>
-      </c>
-      <c r="H4" s="17">
-        <f t="shared" ref="H4:H42" si="0">AVERAGE(F4:G4)</f>
+      <c r="F4" s="26">
         <v>15.7</v>
       </c>
-      <c r="I4" s="26">
-        <f t="shared" ref="I4:I42" si="1">H4+274.15</f>
+      <c r="G4" s="26">
+        <f t="shared" ref="G4:G42" si="0">F4+274.15</f>
         <v>289.84999999999997</v>
       </c>
-      <c r="J4" s="106">
+      <c r="H4" s="106">
         <v>25</v>
       </c>
-      <c r="K4" s="116">
+      <c r="I4" s="116">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L4" s="27">
-        <v>40.200000000000003</v>
-      </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="119"/>
-      <c r="O4" s="159"/>
-      <c r="S4" s="164"/>
+      <c r="J4" s="27">
+        <v>40.4</v>
+      </c>
+      <c r="K4" s="17">
+        <v>55.4</v>
+      </c>
+      <c r="L4" s="119">
+        <v>8.1700000000000002E-3</v>
+      </c>
+      <c r="M4" s="159"/>
+      <c r="N4" s="162"/>
+      <c r="O4" s="162"/>
+      <c r="S4" s="167"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="137"/>
@@ -4888,32 +4997,31 @@
       <c r="E5" s="111">
         <v>6</v>
       </c>
-      <c r="F5" s="27">
-        <v>14.7</v>
-      </c>
-      <c r="G5" s="17">
-        <v>14</v>
-      </c>
-      <c r="H5" s="17">
+      <c r="F5" s="26">
+        <v>14.35</v>
+      </c>
+      <c r="G5" s="26">
         <f t="shared" si="0"/>
-        <v>14.35</v>
-      </c>
-      <c r="I5" s="26">
-        <f t="shared" si="1"/>
         <v>288.5</v>
       </c>
-      <c r="J5" s="106">
+      <c r="H5" s="106">
         <v>25</v>
       </c>
-      <c r="K5" s="116">
+      <c r="I5" s="116">
         <v>0.32</v>
       </c>
-      <c r="L5" s="27">
+      <c r="J5" s="27">
         <v>30</v>
       </c>
-      <c r="M5" s="17"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="159"/>
+      <c r="K5" s="17">
+        <v>45</v>
+      </c>
+      <c r="L5" s="119">
+        <v>1.2370000000000001E-2</v>
+      </c>
+      <c r="M5" s="159"/>
+      <c r="N5" s="162"/>
+      <c r="O5" s="162"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="137"/>
@@ -4925,32 +5033,31 @@
       <c r="E6" s="111">
         <v>7</v>
       </c>
-      <c r="F6" s="27">
-        <v>14.9</v>
-      </c>
-      <c r="G6" s="17">
-        <v>15.3</v>
-      </c>
-      <c r="H6" s="17">
+      <c r="F6" s="26">
+        <v>15.100000000000001</v>
+      </c>
+      <c r="G6" s="26">
         <f t="shared" si="0"/>
-        <v>15.100000000000001</v>
-      </c>
-      <c r="I6" s="26">
-        <f t="shared" si="1"/>
         <v>289.25</v>
       </c>
-      <c r="J6" s="106">
+      <c r="H6" s="106">
         <v>25</v>
       </c>
-      <c r="K6" s="116">
+      <c r="I6" s="116">
         <v>0.32</v>
       </c>
-      <c r="L6" s="27">
+      <c r="J6" s="27">
         <v>30</v>
       </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="119"/>
-      <c r="O6" s="159"/>
+      <c r="K6" s="17">
+        <v>45</v>
+      </c>
+      <c r="L6" s="119">
+        <v>1.6760000000000001E-2</v>
+      </c>
+      <c r="M6" s="159"/>
+      <c r="N6" s="162"/>
+      <c r="O6" s="162"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="150"/>
@@ -4962,78 +5069,82 @@
       <c r="E7" s="131">
         <v>8</v>
       </c>
-      <c r="F7" s="132">
-        <v>15.32</v>
-      </c>
-      <c r="G7" s="68">
-        <v>14.4</v>
-      </c>
-      <c r="H7" s="68">
+      <c r="F7" s="93">
+        <v>14.86</v>
+      </c>
+      <c r="G7" s="133">
         <f t="shared" si="0"/>
-        <v>14.86</v>
-      </c>
-      <c r="I7" s="133">
-        <f t="shared" si="1"/>
         <v>289.01</v>
       </c>
-      <c r="J7" s="134">
+      <c r="H7" s="134">
         <v>25</v>
       </c>
-      <c r="K7" s="135">
+      <c r="I7" s="135">
         <v>0.31</v>
       </c>
-      <c r="L7" s="132">
+      <c r="J7" s="132">
         <v>20.2</v>
       </c>
-      <c r="M7" s="68"/>
-      <c r="N7" s="136"/>
-      <c r="O7" s="160"/>
+      <c r="K7" s="68">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="L7" s="136">
+        <v>7.92E-3</v>
+      </c>
+      <c r="M7" s="160"/>
+      <c r="N7" s="163"/>
+      <c r="O7" s="163"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="161">
+      <c r="A8" s="164">
         <v>2</v>
       </c>
       <c r="B8" s="122">
         <v>1</v>
       </c>
-      <c r="C8" s="162">
+      <c r="C8" s="165">
         <v>20</v>
       </c>
-      <c r="D8" s="162">
-        <f t="shared" ref="D8" si="2">C8+273.15</f>
+      <c r="D8" s="165">
+        <f t="shared" ref="D8" si="1">C8+273.15</f>
         <v>293.14999999999998</v>
       </c>
       <c r="E8" s="123">
         <v>48</v>
       </c>
-      <c r="F8" s="124">
-        <v>19.3</v>
-      </c>
-      <c r="G8" s="125">
-        <v>18.7</v>
-      </c>
-      <c r="H8" s="125">
-        <f>AVERAGE(F8:G8)</f>
+      <c r="F8" s="26">
         <v>19</v>
       </c>
-      <c r="I8" s="126">
-        <f t="shared" si="1"/>
+      <c r="G8" s="126">
+        <f t="shared" si="0"/>
         <v>293.14999999999998</v>
       </c>
-      <c r="J8" s="127">
+      <c r="H8" s="127">
         <v>25</v>
       </c>
-      <c r="K8" s="128">
+      <c r="I8" s="128">
         <v>0.3</v>
       </c>
-      <c r="L8" s="124">
+      <c r="J8" s="124">
         <v>31.8</v>
       </c>
-      <c r="M8" s="125"/>
-      <c r="N8" s="129"/>
-      <c r="O8" s="158" t="e">
-        <f t="shared" ref="O8" si="3">AVERAGE(N8:N12)</f>
-        <v>#DIV/0!</v>
+      <c r="K8" s="125">
+        <v>46.8</v>
+      </c>
+      <c r="L8" s="129">
+        <v>1.397E-2</v>
+      </c>
+      <c r="M8" s="158">
+        <f t="shared" ref="M8" si="2">AVERAGE(L8:L12)</f>
+        <v>1.4062E-2</v>
+      </c>
+      <c r="N8" s="161">
+        <f t="shared" ref="N8" si="3">O8/SQRT(5)</f>
+        <v>2.2252806564566183E-3</v>
+      </c>
+      <c r="O8" s="161">
+        <f t="shared" ref="O8" si="4">_xlfn.STDEV.S(L8:L12)</f>
+        <v>4.9758788168523553E-3</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -5046,32 +5157,31 @@
       <c r="E9" s="111">
         <v>9</v>
       </c>
-      <c r="F9" s="27">
-        <v>21.4</v>
-      </c>
-      <c r="G9" s="17">
-        <v>20.5</v>
-      </c>
-      <c r="H9" s="17">
-        <f>AVERAGE(F9:G9)</f>
+      <c r="F9" s="26">
         <v>20.95</v>
       </c>
-      <c r="I9" s="26">
-        <f t="shared" si="1"/>
+      <c r="G9" s="26">
+        <f t="shared" si="0"/>
         <v>295.09999999999997</v>
       </c>
-      <c r="J9" s="107">
+      <c r="H9" s="107">
         <v>25</v>
       </c>
-      <c r="K9" s="116">
+      <c r="I9" s="116">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L9" s="27">
+      <c r="J9" s="27">
         <v>17.2</v>
       </c>
-      <c r="M9" s="17"/>
-      <c r="N9" s="119"/>
-      <c r="O9" s="159"/>
+      <c r="K9" s="17">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="L9" s="119">
+        <v>8.6400000000000001E-3</v>
+      </c>
+      <c r="M9" s="159"/>
+      <c r="N9" s="162"/>
+      <c r="O9" s="162"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="137"/>
@@ -5083,32 +5193,31 @@
       <c r="E10" s="111">
         <v>10</v>
       </c>
-      <c r="F10" s="27">
-        <v>21</v>
-      </c>
-      <c r="G10" s="17">
-        <v>21.3</v>
-      </c>
-      <c r="H10" s="17">
-        <f>AVERAGE(F10:G10)</f>
+      <c r="F10" s="26">
         <v>21.15</v>
       </c>
-      <c r="I10" s="26">
-        <f t="shared" si="1"/>
+      <c r="G10" s="26">
+        <f t="shared" si="0"/>
         <v>295.29999999999995</v>
       </c>
-      <c r="J10" s="107">
+      <c r="H10" s="107">
         <v>25</v>
       </c>
-      <c r="K10" s="116">
+      <c r="I10" s="116">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L10" s="27">
+      <c r="J10" s="27">
         <v>25.8</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" s="119"/>
-      <c r="O10" s="159"/>
+      <c r="K10" s="17">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="L10" s="119">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="M10" s="159"/>
+      <c r="N10" s="162"/>
+      <c r="O10" s="162"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="137"/>
@@ -5120,32 +5229,31 @@
       <c r="E11" s="111">
         <v>11</v>
       </c>
-      <c r="F11" s="27">
-        <v>19.7</v>
-      </c>
-      <c r="G11" s="17">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="H11" s="17">
-        <f>AVERAGE(F11:G11)</f>
+      <c r="F11" s="26">
         <v>19.549999999999997</v>
       </c>
-      <c r="I11" s="26">
-        <f t="shared" si="1"/>
+      <c r="G11" s="26">
+        <f t="shared" si="0"/>
         <v>293.7</v>
       </c>
-      <c r="J11" s="107">
+      <c r="H11" s="107">
         <v>25</v>
       </c>
-      <c r="K11" s="116">
+      <c r="I11" s="116">
         <v>0.31</v>
       </c>
-      <c r="L11" s="27">
+      <c r="J11" s="27">
         <v>30</v>
       </c>
-      <c r="M11" s="17"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="159"/>
+      <c r="K11" s="17">
+        <v>45</v>
+      </c>
+      <c r="L11" s="119">
+        <v>2.171E-2</v>
+      </c>
+      <c r="M11" s="159"/>
+      <c r="N11" s="162"/>
+      <c r="O11" s="162"/>
     </row>
     <row r="12" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="150"/>
@@ -5157,78 +5265,82 @@
       <c r="E12" s="113">
         <v>12</v>
       </c>
-      <c r="F12" s="29">
-        <v>19.3</v>
-      </c>
-      <c r="G12" s="18">
-        <v>19.8</v>
-      </c>
-      <c r="H12" s="18">
-        <f>AVERAGE(F12:G12)</f>
+      <c r="F12" s="26">
         <v>19.55</v>
       </c>
-      <c r="I12" s="103">
-        <f t="shared" si="1"/>
+      <c r="G12" s="103">
+        <f t="shared" si="0"/>
         <v>293.7</v>
       </c>
-      <c r="J12" s="108">
+      <c r="H12" s="108">
         <v>25</v>
       </c>
-      <c r="K12" s="118">
+      <c r="I12" s="118">
         <v>0.31</v>
       </c>
-      <c r="L12" s="29">
+      <c r="J12" s="29">
         <v>24</v>
       </c>
-      <c r="M12" s="18"/>
-      <c r="N12" s="120"/>
-      <c r="O12" s="160"/>
+      <c r="K12" s="18">
+        <v>39</v>
+      </c>
+      <c r="L12" s="120">
+        <v>1.089E-2</v>
+      </c>
+      <c r="M12" s="160"/>
+      <c r="N12" s="163"/>
+      <c r="O12" s="163"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="161">
+      <c r="A13" s="164">
         <v>3</v>
       </c>
       <c r="B13" s="122">
         <v>1</v>
       </c>
-      <c r="C13" s="162">
+      <c r="C13" s="165">
         <v>25</v>
       </c>
-      <c r="D13" s="162">
-        <f t="shared" ref="D13" si="4">C13+273.15</f>
+      <c r="D13" s="165">
+        <f t="shared" ref="D13" si="5">C13+273.15</f>
         <v>298.14999999999998</v>
       </c>
       <c r="E13" s="123">
         <v>13</v>
       </c>
-      <c r="F13" s="124">
-        <v>25.2</v>
-      </c>
-      <c r="G13" s="125">
-        <v>25.8</v>
-      </c>
-      <c r="H13" s="125">
+      <c r="F13" s="26">
+        <v>25.5</v>
+      </c>
+      <c r="G13" s="126">
         <f t="shared" si="0"/>
-        <v>25.5</v>
-      </c>
-      <c r="I13" s="126">
-        <f t="shared" si="1"/>
         <v>299.64999999999998</v>
       </c>
-      <c r="J13" s="127">
+      <c r="H13" s="127">
         <v>25</v>
       </c>
-      <c r="K13" s="128">
+      <c r="I13" s="128">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L13" s="124">
+      <c r="J13" s="124">
         <v>19</v>
       </c>
-      <c r="M13" s="125"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="158" t="e">
-        <f t="shared" ref="O13" si="5">AVERAGE(N13:N17)</f>
-        <v>#DIV/0!</v>
+      <c r="K13" s="125">
+        <v>34</v>
+      </c>
+      <c r="L13" s="129">
+        <v>1.8669999999999999E-2</v>
+      </c>
+      <c r="M13" s="158">
+        <f t="shared" ref="M13" si="6">AVERAGE(L13:L17)</f>
+        <v>1.7819999999999996E-2</v>
+      </c>
+      <c r="N13" s="161">
+        <f t="shared" ref="N13" si="7">O13/SQRT(5)</f>
+        <v>3.1548993644805894E-3</v>
+      </c>
+      <c r="O13" s="161">
+        <f t="shared" ref="O13" si="8">_xlfn.STDEV.S(L13:L17)</f>
+        <v>7.0545694411494834E-3</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -5241,32 +5353,31 @@
       <c r="E14" s="111">
         <v>14</v>
       </c>
-      <c r="F14" s="27">
-        <v>25.3</v>
-      </c>
-      <c r="G14" s="17">
-        <v>25.8</v>
-      </c>
-      <c r="H14" s="17">
+      <c r="F14" s="26">
+        <v>25.55</v>
+      </c>
+      <c r="G14" s="26">
         <f t="shared" si="0"/>
-        <v>25.55</v>
-      </c>
-      <c r="I14" s="26">
-        <f t="shared" si="1"/>
         <v>299.7</v>
       </c>
-      <c r="J14" s="107">
+      <c r="H14" s="107">
         <v>25</v>
       </c>
-      <c r="K14" s="116">
+      <c r="I14" s="116">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L14" s="27">
+      <c r="J14" s="27">
         <v>20</v>
       </c>
-      <c r="M14" s="17"/>
-      <c r="N14" s="119"/>
-      <c r="O14" s="159"/>
+      <c r="K14" s="17">
+        <v>35</v>
+      </c>
+      <c r="L14" s="119">
+        <v>2.8639999999999999E-2</v>
+      </c>
+      <c r="M14" s="159"/>
+      <c r="N14" s="162"/>
+      <c r="O14" s="162"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="137"/>
@@ -5278,32 +5389,31 @@
       <c r="E15" s="111">
         <v>15</v>
       </c>
-      <c r="F15" s="27">
-        <v>25.7</v>
-      </c>
-      <c r="G15" s="17">
-        <v>26.7</v>
-      </c>
-      <c r="H15" s="17">
+      <c r="F15" s="26">
+        <v>26.2</v>
+      </c>
+      <c r="G15" s="26">
         <f t="shared" si="0"/>
-        <v>26.2</v>
-      </c>
-      <c r="I15" s="26">
-        <f t="shared" si="1"/>
         <v>300.34999999999997</v>
       </c>
-      <c r="J15" s="107">
+      <c r="H15" s="107">
         <v>25</v>
       </c>
-      <c r="K15" s="116">
+      <c r="I15" s="116">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L15" s="27">
+      <c r="J15" s="27">
         <v>27.2</v>
       </c>
-      <c r="M15" s="17"/>
-      <c r="N15" s="119"/>
-      <c r="O15" s="159"/>
+      <c r="K15" s="17">
+        <v>42.2</v>
+      </c>
+      <c r="L15" s="119">
+        <v>1.6310000000000002E-2</v>
+      </c>
+      <c r="M15" s="159"/>
+      <c r="N15" s="162"/>
+      <c r="O15" s="162"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="137"/>
@@ -5315,32 +5425,31 @@
       <c r="E16" s="111">
         <v>16</v>
       </c>
-      <c r="F16" s="27">
-        <v>24.7</v>
-      </c>
-      <c r="G16" s="17">
-        <v>24.6</v>
-      </c>
-      <c r="H16" s="17">
+      <c r="F16" s="26">
+        <v>24.65</v>
+      </c>
+      <c r="G16" s="26">
         <f t="shared" si="0"/>
-        <v>24.65</v>
-      </c>
-      <c r="I16" s="26">
-        <f t="shared" si="1"/>
         <v>298.79999999999995</v>
       </c>
-      <c r="J16" s="107">
+      <c r="H16" s="107">
         <v>25</v>
       </c>
-      <c r="K16" s="116">
+      <c r="I16" s="116">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L16" s="27">
+      <c r="J16" s="27">
         <v>24</v>
       </c>
-      <c r="M16" s="17"/>
-      <c r="N16" s="119"/>
-      <c r="O16" s="159"/>
+      <c r="K16" s="17">
+        <v>39</v>
+      </c>
+      <c r="L16" s="119">
+        <v>1.644E-2</v>
+      </c>
+      <c r="M16" s="159"/>
+      <c r="N16" s="162"/>
+      <c r="O16" s="162"/>
     </row>
     <row r="17" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="150"/>
@@ -5352,78 +5461,82 @@
       <c r="E17" s="113">
         <v>17</v>
       </c>
-      <c r="F17" s="29">
-        <v>25.4</v>
-      </c>
-      <c r="G17" s="18">
-        <v>25.9</v>
-      </c>
-      <c r="H17" s="18">
+      <c r="F17" s="26">
+        <v>25.65</v>
+      </c>
+      <c r="G17" s="103">
         <f t="shared" si="0"/>
-        <v>25.65</v>
-      </c>
-      <c r="I17" s="103">
-        <f t="shared" si="1"/>
         <v>299.79999999999995</v>
       </c>
-      <c r="J17" s="108">
+      <c r="H17" s="108">
         <v>25</v>
       </c>
-      <c r="K17" s="118">
+      <c r="I17" s="118">
         <v>0.3</v>
       </c>
-      <c r="L17" s="29">
+      <c r="J17" s="29">
         <v>20</v>
       </c>
-      <c r="M17" s="18"/>
-      <c r="N17" s="120"/>
-      <c r="O17" s="160"/>
+      <c r="K17" s="18">
+        <v>35</v>
+      </c>
+      <c r="L17" s="120">
+        <v>9.0399999999999994E-3</v>
+      </c>
+      <c r="M17" s="160"/>
+      <c r="N17" s="163"/>
+      <c r="O17" s="163"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="161">
+      <c r="A18" s="164">
         <v>4</v>
       </c>
       <c r="B18" s="122">
         <v>1</v>
       </c>
-      <c r="C18" s="162">
+      <c r="C18" s="165">
         <v>30</v>
       </c>
-      <c r="D18" s="162">
-        <f t="shared" ref="D18" si="6">C18+273.15</f>
+      <c r="D18" s="165">
+        <f t="shared" ref="D18" si="9">C18+273.15</f>
         <v>303.14999999999998</v>
       </c>
       <c r="E18" s="123">
         <v>18</v>
       </c>
-      <c r="F18" s="124">
-        <v>29.6</v>
-      </c>
-      <c r="G18" s="125">
-        <v>30.6</v>
-      </c>
-      <c r="H18" s="125">
-        <f>AVERAGE(F18:G18)</f>
+      <c r="F18" s="26">
         <v>30.1</v>
       </c>
-      <c r="I18" s="126">
-        <f t="shared" si="1"/>
+      <c r="G18" s="126">
+        <f t="shared" si="0"/>
         <v>304.25</v>
       </c>
-      <c r="J18" s="127">
+      <c r="H18" s="127">
         <v>25</v>
       </c>
-      <c r="K18" s="128">
+      <c r="I18" s="128">
         <v>0.33</v>
       </c>
-      <c r="L18" s="124">
-        <v>56</v>
-      </c>
-      <c r="M18" s="125"/>
-      <c r="N18" s="129"/>
-      <c r="O18" s="158" t="e">
-        <f t="shared" ref="O18" si="7">AVERAGE(N18:N22)</f>
-        <v>#DIV/0!</v>
+      <c r="J18" s="124">
+        <v>5.6</v>
+      </c>
+      <c r="K18" s="125">
+        <v>20.6</v>
+      </c>
+      <c r="L18" s="129">
+        <v>3.8109999999999998E-2</v>
+      </c>
+      <c r="M18" s="158">
+        <f t="shared" ref="M18" si="10">AVERAGE(L18:L22)</f>
+        <v>3.8837999999999998E-2</v>
+      </c>
+      <c r="N18" s="161">
+        <f t="shared" ref="N18" si="11">O18/SQRT(5)</f>
+        <v>8.6950131684776603E-3</v>
+      </c>
+      <c r="O18" s="161">
+        <f t="shared" ref="O18" si="12">_xlfn.STDEV.S(L18:L22)</f>
+        <v>1.9442640509971881E-2</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
@@ -5436,32 +5549,31 @@
       <c r="E19" s="111">
         <v>19</v>
       </c>
-      <c r="F19" s="27">
-        <v>29.1</v>
-      </c>
-      <c r="G19" s="17">
-        <v>28.5</v>
-      </c>
-      <c r="H19" s="17">
-        <f>AVERAGE(F19:G19)</f>
+      <c r="F19" s="26">
         <v>28.8</v>
       </c>
-      <c r="I19" s="26">
-        <f t="shared" si="1"/>
+      <c r="G19" s="26">
+        <f t="shared" si="0"/>
         <v>302.95</v>
       </c>
-      <c r="J19" s="107">
+      <c r="H19" s="107">
         <v>25</v>
       </c>
-      <c r="K19" s="116">
+      <c r="I19" s="116">
         <v>0.3</v>
       </c>
-      <c r="L19" s="27">
+      <c r="J19" s="27">
         <v>10.199999999999999</v>
       </c>
-      <c r="M19" s="17"/>
-      <c r="N19" s="119"/>
-      <c r="O19" s="159"/>
+      <c r="K19" s="17">
+        <v>25.2</v>
+      </c>
+      <c r="L19" s="119">
+        <v>2.3269999999999999E-2</v>
+      </c>
+      <c r="M19" s="159"/>
+      <c r="N19" s="162"/>
+      <c r="O19" s="162"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="137"/>
@@ -5473,32 +5585,31 @@
       <c r="E20" s="111">
         <v>20</v>
       </c>
-      <c r="F20" s="27">
-        <v>30.9</v>
-      </c>
-      <c r="G20" s="17">
-        <v>31.5</v>
-      </c>
-      <c r="H20" s="17">
-        <f>AVERAGE(F20:G20)</f>
+      <c r="F20" s="26">
         <v>31.2</v>
       </c>
-      <c r="I20" s="26">
-        <f t="shared" si="1"/>
+      <c r="G20" s="26">
+        <f t="shared" si="0"/>
         <v>305.34999999999997</v>
       </c>
-      <c r="J20" s="107">
+      <c r="H20" s="107">
         <v>25</v>
       </c>
-      <c r="K20" s="116">
+      <c r="I20" s="116">
         <v>0.3</v>
       </c>
-      <c r="L20" s="27">
+      <c r="J20" s="27">
         <v>11</v>
       </c>
-      <c r="M20" s="17"/>
-      <c r="N20" s="119"/>
-      <c r="O20" s="159"/>
+      <c r="K20" s="17">
+        <v>26</v>
+      </c>
+      <c r="L20" s="119">
+        <v>6.7760000000000001E-2</v>
+      </c>
+      <c r="M20" s="159"/>
+      <c r="N20" s="162"/>
+      <c r="O20" s="162"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="137"/>
@@ -5510,32 +5621,31 @@
       <c r="E21" s="111">
         <v>21</v>
       </c>
-      <c r="F21" s="27">
-        <v>30</v>
-      </c>
-      <c r="G21" s="17">
-        <v>30.4</v>
-      </c>
-      <c r="H21" s="17">
-        <f>AVERAGE(F21:G21)</f>
+      <c r="F21" s="26">
         <v>30.2</v>
       </c>
-      <c r="I21" s="26">
-        <f t="shared" si="1"/>
+      <c r="G21" s="26">
+        <f t="shared" si="0"/>
         <v>304.34999999999997</v>
       </c>
-      <c r="J21" s="107">
+      <c r="H21" s="107">
         <v>25</v>
       </c>
-      <c r="K21" s="116">
+      <c r="I21" s="116">
         <v>0.3</v>
       </c>
-      <c r="L21" s="27">
+      <c r="J21" s="27">
         <v>17.2</v>
       </c>
-      <c r="M21" s="17"/>
-      <c r="N21" s="119"/>
-      <c r="O21" s="159"/>
+      <c r="K21" s="17">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="L21" s="119">
+        <v>4.5809999999999997E-2</v>
+      </c>
+      <c r="M21" s="159"/>
+      <c r="N21" s="162"/>
+      <c r="O21" s="162"/>
     </row>
     <row r="22" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="150"/>
@@ -5547,78 +5657,82 @@
       <c r="E22" s="113">
         <v>22</v>
       </c>
-      <c r="F22" s="29">
-        <v>30.8</v>
-      </c>
-      <c r="G22" s="18">
-        <v>31</v>
-      </c>
-      <c r="H22" s="18">
-        <f>AVERAGE(F22:G22)</f>
+      <c r="F22" s="26">
         <v>30.9</v>
       </c>
-      <c r="I22" s="103">
-        <f t="shared" si="1"/>
+      <c r="G22" s="103">
+        <f t="shared" si="0"/>
         <v>305.04999999999995</v>
       </c>
-      <c r="J22" s="108">
+      <c r="H22" s="108">
         <v>25</v>
       </c>
-      <c r="K22" s="118">
+      <c r="I22" s="118">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L22" s="29">
+      <c r="J22" s="29">
         <v>11.4</v>
       </c>
-      <c r="M22" s="18"/>
-      <c r="N22" s="120"/>
-      <c r="O22" s="160"/>
+      <c r="K22" s="18">
+        <v>26.4</v>
+      </c>
+      <c r="L22" s="120">
+        <v>1.924E-2</v>
+      </c>
+      <c r="M22" s="160"/>
+      <c r="N22" s="163"/>
+      <c r="O22" s="163"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="161">
+      <c r="A23" s="164">
         <v>5</v>
       </c>
       <c r="B23" s="122">
         <v>1</v>
       </c>
-      <c r="C23" s="162">
+      <c r="C23" s="165">
         <v>35</v>
       </c>
-      <c r="D23" s="162">
-        <f t="shared" ref="D23" si="8">C23+273.15</f>
+      <c r="D23" s="165">
+        <f t="shared" ref="D23" si="13">C23+273.15</f>
         <v>308.14999999999998</v>
       </c>
       <c r="E23" s="123">
         <v>23</v>
       </c>
-      <c r="F23" s="124">
-        <v>35.6</v>
-      </c>
-      <c r="G23" s="125">
-        <v>35.4</v>
-      </c>
-      <c r="H23" s="125">
+      <c r="F23" s="26">
+        <v>35.5</v>
+      </c>
+      <c r="G23" s="126">
         <f t="shared" si="0"/>
-        <v>35.5</v>
-      </c>
-      <c r="I23" s="126">
-        <f t="shared" si="1"/>
         <v>309.64999999999998</v>
       </c>
-      <c r="J23" s="127">
+      <c r="H23" s="127">
         <v>25</v>
       </c>
-      <c r="K23" s="128">
+      <c r="I23" s="128">
         <v>0.31</v>
       </c>
-      <c r="L23" s="124">
+      <c r="J23" s="124">
         <v>8</v>
       </c>
-      <c r="M23" s="125"/>
-      <c r="N23" s="129"/>
-      <c r="O23" s="158" t="e">
-        <f t="shared" ref="O23" si="9">AVERAGE(N23:N27)</f>
-        <v>#DIV/0!</v>
+      <c r="K23" s="125">
+        <v>23</v>
+      </c>
+      <c r="L23" s="129">
+        <v>6.9919999999999996E-2</v>
+      </c>
+      <c r="M23" s="158">
+        <f t="shared" ref="M23" si="14">AVERAGE(L23:L27)</f>
+        <v>5.4418000000000001E-2</v>
+      </c>
+      <c r="N23" s="161">
+        <f t="shared" ref="N23" si="15">O23/SQRT(5)</f>
+        <v>6.0011560552946722E-3</v>
+      </c>
+      <c r="O23" s="161">
+        <f t="shared" ref="O23" si="16">_xlfn.STDEV.S(L23:L27)</f>
+        <v>1.3418992883223374E-2</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5631,32 +5745,31 @@
       <c r="E24" s="111">
         <v>24</v>
       </c>
-      <c r="F24" s="27">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="G24" s="17">
-        <v>35.799999999999997</v>
-      </c>
-      <c r="H24" s="17">
+      <c r="F24" s="26">
+        <v>35.549999999999997</v>
+      </c>
+      <c r="G24" s="26">
         <f t="shared" si="0"/>
-        <v>35.549999999999997</v>
-      </c>
-      <c r="I24" s="26">
-        <f t="shared" si="1"/>
         <v>309.7</v>
       </c>
-      <c r="J24" s="107">
+      <c r="H24" s="107">
         <v>25</v>
       </c>
-      <c r="K24" s="116">
+      <c r="I24" s="116">
         <v>0.31</v>
       </c>
-      <c r="L24" s="27">
+      <c r="J24" s="27">
         <v>16.8</v>
       </c>
-      <c r="M24" s="17"/>
-      <c r="N24" s="119"/>
-      <c r="O24" s="159"/>
+      <c r="K24" s="17">
+        <v>31.8</v>
+      </c>
+      <c r="L24" s="119">
+        <v>5.917E-2</v>
+      </c>
+      <c r="M24" s="159"/>
+      <c r="N24" s="162"/>
+      <c r="O24" s="162"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="137"/>
@@ -5668,32 +5781,31 @@
       <c r="E25" s="111">
         <v>25</v>
       </c>
-      <c r="F25" s="27">
-        <v>35.1</v>
-      </c>
-      <c r="G25" s="17">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="H25" s="17">
+      <c r="F25" s="26">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="G25" s="26">
         <f t="shared" si="0"/>
-        <v>34.200000000000003</v>
-      </c>
-      <c r="I25" s="26">
-        <f t="shared" si="1"/>
         <v>308.34999999999997</v>
       </c>
-      <c r="J25" s="107">
+      <c r="H25" s="107">
         <v>25</v>
       </c>
-      <c r="K25" s="116">
+      <c r="I25" s="116">
         <v>0.32</v>
       </c>
-      <c r="L25" s="27">
+      <c r="J25" s="27">
         <v>13.2</v>
       </c>
-      <c r="M25" s="17"/>
-      <c r="N25" s="119"/>
-      <c r="O25" s="159"/>
+      <c r="K25" s="17">
+        <v>28.2</v>
+      </c>
+      <c r="L25" s="119">
+        <v>6.2269999999999999E-2</v>
+      </c>
+      <c r="M25" s="159"/>
+      <c r="N25" s="162"/>
+      <c r="O25" s="162"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="137"/>
@@ -5705,32 +5817,31 @@
       <c r="E26" s="111">
         <v>26</v>
       </c>
-      <c r="F26" s="27">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="G26" s="17">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="H26" s="17">
+      <c r="F26" s="26">
+        <v>35</v>
+      </c>
+      <c r="G26" s="26">
         <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="I26" s="26">
-        <f t="shared" si="1"/>
         <v>309.14999999999998</v>
       </c>
-      <c r="J26" s="107">
+      <c r="H26" s="107">
         <v>25</v>
       </c>
-      <c r="K26" s="116">
+      <c r="I26" s="116">
         <v>0.31</v>
       </c>
-      <c r="L26" s="27">
+      <c r="J26" s="27">
         <v>6.2</v>
       </c>
-      <c r="M26" s="17"/>
-      <c r="N26" s="119"/>
-      <c r="O26" s="159"/>
+      <c r="K26" s="17">
+        <v>21.2</v>
+      </c>
+      <c r="L26" s="119">
+        <v>4.0980000000000003E-2</v>
+      </c>
+      <c r="M26" s="159"/>
+      <c r="N26" s="162"/>
+      <c r="O26" s="162"/>
     </row>
     <row r="27" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="150"/>
@@ -5742,78 +5853,82 @@
       <c r="E27" s="113">
         <v>27</v>
       </c>
-      <c r="F27" s="29">
-        <v>35.5</v>
-      </c>
-      <c r="G27" s="18">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="H27" s="18">
+      <c r="F27" s="26">
+        <v>35.9</v>
+      </c>
+      <c r="G27" s="103">
         <f t="shared" si="0"/>
-        <v>35.9</v>
-      </c>
-      <c r="I27" s="103">
-        <f t="shared" si="1"/>
         <v>310.04999999999995</v>
       </c>
-      <c r="J27" s="108">
+      <c r="H27" s="108">
         <v>25</v>
       </c>
-      <c r="K27" s="118">
+      <c r="I27" s="118">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L27" s="29">
+      <c r="J27" s="29">
         <v>21.4</v>
       </c>
-      <c r="M27" s="18"/>
-      <c r="N27" s="120"/>
-      <c r="O27" s="160"/>
+      <c r="K27" s="18">
+        <v>36.4</v>
+      </c>
+      <c r="L27" s="120">
+        <v>3.9750000000000001E-2</v>
+      </c>
+      <c r="M27" s="160"/>
+      <c r="N27" s="163"/>
+      <c r="O27" s="163"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="161">
+      <c r="A28" s="164">
         <v>6</v>
       </c>
       <c r="B28" s="122">
         <v>1</v>
       </c>
-      <c r="C28" s="162">
+      <c r="C28" s="165">
         <v>40</v>
       </c>
-      <c r="D28" s="162">
-        <f t="shared" ref="D28" si="10">C28+273.15</f>
+      <c r="D28" s="165">
+        <f t="shared" ref="D28" si="17">C28+273.15</f>
         <v>313.14999999999998</v>
       </c>
       <c r="E28" s="123">
         <v>43</v>
       </c>
-      <c r="F28" s="124">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="G28" s="125">
-        <v>40.9</v>
-      </c>
-      <c r="H28" s="125">
+      <c r="F28" s="26">
+        <v>40.349999999999994</v>
+      </c>
+      <c r="G28" s="126">
         <f t="shared" si="0"/>
-        <v>40.349999999999994</v>
-      </c>
-      <c r="I28" s="126">
-        <f t="shared" si="1"/>
         <v>314.5</v>
       </c>
-      <c r="J28" s="127">
+      <c r="H28" s="127">
         <v>25</v>
       </c>
-      <c r="K28" s="128">
+      <c r="I28" s="128">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L28" s="124">
+      <c r="J28" s="124">
         <v>11.6</v>
       </c>
-      <c r="M28" s="125"/>
-      <c r="N28" s="129"/>
-      <c r="O28" s="158" t="e">
-        <f t="shared" ref="O28" si="11">AVERAGE(N28:N32)</f>
-        <v>#DIV/0!</v>
+      <c r="K28" s="125">
+        <v>26.6</v>
+      </c>
+      <c r="L28" s="129">
+        <v>6.0900000000000003E-2</v>
+      </c>
+      <c r="M28" s="158">
+        <f t="shared" ref="M28" si="18">AVERAGE(L28:L32)</f>
+        <v>4.2141999999999999E-2</v>
+      </c>
+      <c r="N28" s="161">
+        <f t="shared" ref="N28" si="19">O28/SQRT(5)</f>
+        <v>8.2617494515387011E-3</v>
+      </c>
+      <c r="O28" s="161">
+        <f t="shared" ref="O28" si="20">_xlfn.STDEV.S(L28:L32)</f>
+        <v>1.847383338671214E-2</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -5826,32 +5941,31 @@
       <c r="E29" s="111">
         <v>44</v>
       </c>
-      <c r="F29" s="27">
-        <v>41.3</v>
-      </c>
-      <c r="G29" s="17">
-        <v>41.1</v>
-      </c>
-      <c r="H29" s="17">
+      <c r="F29" s="26">
+        <v>41.2</v>
+      </c>
+      <c r="G29" s="26">
         <f t="shared" si="0"/>
-        <v>41.2</v>
-      </c>
-      <c r="I29" s="26">
-        <f t="shared" si="1"/>
         <v>315.34999999999997</v>
       </c>
-      <c r="J29" s="107">
+      <c r="H29" s="107">
         <v>25</v>
       </c>
-      <c r="K29" s="116">
+      <c r="I29" s="116">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L29" s="27">
+      <c r="J29" s="27">
         <v>11</v>
       </c>
-      <c r="M29" s="17"/>
-      <c r="N29" s="119"/>
-      <c r="O29" s="159"/>
+      <c r="K29" s="17">
+        <v>26</v>
+      </c>
+      <c r="L29" s="119">
+        <v>2.9139999999999999E-2</v>
+      </c>
+      <c r="M29" s="159"/>
+      <c r="N29" s="162"/>
+      <c r="O29" s="162"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="137"/>
@@ -5863,32 +5977,31 @@
       <c r="E30" s="111">
         <v>45</v>
       </c>
-      <c r="F30" s="27">
-        <v>40.5</v>
-      </c>
-      <c r="G30" s="17">
-        <v>37.299999999999997</v>
-      </c>
-      <c r="H30" s="17">
+      <c r="F30" s="26">
+        <v>38.9</v>
+      </c>
+      <c r="G30" s="26">
         <f t="shared" si="0"/>
-        <v>38.9</v>
-      </c>
-      <c r="I30" s="26">
-        <f t="shared" si="1"/>
         <v>313.04999999999995</v>
       </c>
-      <c r="J30" s="107">
+      <c r="H30" s="107">
         <v>25</v>
       </c>
-      <c r="K30" s="116">
+      <c r="I30" s="116">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L30" s="27">
+      <c r="J30" s="27">
         <v>9.6</v>
       </c>
-      <c r="M30" s="17"/>
-      <c r="N30" s="119"/>
-      <c r="O30" s="159"/>
+      <c r="K30" s="17">
+        <v>24.6</v>
+      </c>
+      <c r="L30" s="119">
+        <v>2.469E-2</v>
+      </c>
+      <c r="M30" s="159"/>
+      <c r="N30" s="162"/>
+      <c r="O30" s="162"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="137"/>
@@ -5900,32 +6013,31 @@
       <c r="E31" s="111">
         <v>46</v>
       </c>
-      <c r="F31" s="27">
-        <v>40</v>
-      </c>
-      <c r="G31" s="17">
-        <v>41</v>
-      </c>
-      <c r="H31" s="17">
+      <c r="F31" s="26">
+        <v>40.5</v>
+      </c>
+      <c r="G31" s="26">
         <f t="shared" si="0"/>
-        <v>40.5</v>
-      </c>
-      <c r="I31" s="26">
-        <f t="shared" si="1"/>
         <v>314.64999999999998</v>
       </c>
-      <c r="J31" s="107">
+      <c r="H31" s="107">
         <v>25</v>
       </c>
-      <c r="K31" s="116">
+      <c r="I31" s="116">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L31" s="27">
+      <c r="J31" s="27">
         <v>8.8000000000000007</v>
       </c>
-      <c r="M31" s="17"/>
-      <c r="N31" s="119"/>
-      <c r="O31" s="159"/>
+      <c r="K31" s="17">
+        <v>23.8</v>
+      </c>
+      <c r="L31" s="119">
+        <v>6.3339999999999994E-2</v>
+      </c>
+      <c r="M31" s="159"/>
+      <c r="N31" s="162"/>
+      <c r="O31" s="162"/>
     </row>
     <row r="32" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="150"/>
@@ -5937,78 +6049,82 @@
       <c r="E32" s="113">
         <v>47</v>
       </c>
-      <c r="F32" s="29">
-        <v>39.1</v>
-      </c>
-      <c r="G32" s="18">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="H32" s="18">
+      <c r="F32" s="26">
+        <v>38.950000000000003</v>
+      </c>
+      <c r="G32" s="103">
         <f t="shared" si="0"/>
-        <v>38.950000000000003</v>
-      </c>
-      <c r="I32" s="103">
-        <f t="shared" si="1"/>
         <v>313.09999999999997</v>
       </c>
-      <c r="J32" s="108">
+      <c r="H32" s="108">
         <v>25</v>
       </c>
-      <c r="K32" s="118">
+      <c r="I32" s="118">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L32" s="29">
-        <v>9.6</v>
-      </c>
-      <c r="M32" s="18"/>
-      <c r="N32" s="120"/>
-      <c r="O32" s="160"/>
+      <c r="J32" s="29">
+        <v>10</v>
+      </c>
+      <c r="K32" s="18">
+        <v>25</v>
+      </c>
+      <c r="L32" s="120">
+        <v>3.2640000000000002E-2</v>
+      </c>
+      <c r="M32" s="160"/>
+      <c r="N32" s="163"/>
+      <c r="O32" s="163"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="161">
+      <c r="A33" s="164">
         <v>7</v>
       </c>
       <c r="B33" s="122">
         <v>1</v>
       </c>
-      <c r="C33" s="162">
+      <c r="C33" s="165">
         <v>45</v>
       </c>
-      <c r="D33" s="162">
-        <f t="shared" ref="D33" si="12">C33+273.15</f>
+      <c r="D33" s="165">
+        <f t="shared" ref="D33" si="21">C33+273.15</f>
         <v>318.14999999999998</v>
       </c>
       <c r="E33" s="123">
         <v>33</v>
       </c>
-      <c r="F33" s="124">
-        <v>45.6</v>
-      </c>
-      <c r="G33" s="125">
-        <v>44.9</v>
-      </c>
-      <c r="H33" s="125">
+      <c r="F33" s="26">
+        <v>45.25</v>
+      </c>
+      <c r="G33" s="126">
         <f t="shared" si="0"/>
-        <v>45.25</v>
-      </c>
-      <c r="I33" s="126">
-        <f t="shared" si="1"/>
         <v>319.39999999999998</v>
       </c>
-      <c r="J33" s="127">
+      <c r="H33" s="127">
         <v>25</v>
       </c>
-      <c r="K33" s="128">
+      <c r="I33" s="128">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L33" s="124">
+      <c r="J33" s="124">
         <v>6.6</v>
       </c>
-      <c r="M33" s="125"/>
-      <c r="N33" s="129"/>
-      <c r="O33" s="158" t="e">
-        <f t="shared" ref="O33" si="13">AVERAGE(N33:N37)</f>
-        <v>#DIV/0!</v>
+      <c r="K33" s="125">
+        <v>21.6</v>
+      </c>
+      <c r="L33" s="129">
+        <v>4.1390000000000003E-2</v>
+      </c>
+      <c r="M33" s="158">
+        <f t="shared" ref="M33" si="22">AVERAGE(L33:L37)</f>
+        <v>9.4269999999999993E-2</v>
+      </c>
+      <c r="N33" s="161">
+        <f t="shared" ref="N33" si="23">O33/SQRT(5)</f>
+        <v>3.0525774846840499E-2</v>
+      </c>
+      <c r="O33" s="161">
+        <f t="shared" ref="O33" si="24">_xlfn.STDEV.S(L33:L37)</f>
+        <v>6.8257707623388592E-2</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
@@ -6021,32 +6137,31 @@
       <c r="E34" s="111">
         <v>34</v>
       </c>
-      <c r="F34" s="27">
-        <v>44.5</v>
-      </c>
-      <c r="G34" s="17">
-        <v>43.2</v>
-      </c>
-      <c r="H34" s="17">
+      <c r="F34" s="26">
+        <v>43.85</v>
+      </c>
+      <c r="G34" s="26">
         <f t="shared" si="0"/>
-        <v>43.85</v>
-      </c>
-      <c r="I34" s="26">
-        <f t="shared" si="1"/>
         <v>318</v>
       </c>
-      <c r="J34" s="107">
+      <c r="H34" s="107">
         <v>25</v>
       </c>
-      <c r="K34" s="116">
+      <c r="I34" s="116">
         <v>0.3</v>
       </c>
-      <c r="L34" s="27">
+      <c r="J34" s="27">
         <v>16.2</v>
       </c>
-      <c r="M34" s="17"/>
-      <c r="N34" s="119"/>
-      <c r="O34" s="159"/>
+      <c r="K34" s="17">
+        <v>31.2</v>
+      </c>
+      <c r="L34" s="119">
+        <v>6.9720000000000004E-2</v>
+      </c>
+      <c r="M34" s="159"/>
+      <c r="N34" s="162"/>
+      <c r="O34" s="162"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="137"/>
@@ -6058,32 +6173,31 @@
       <c r="E35" s="111">
         <v>35</v>
       </c>
-      <c r="F35" s="27">
+      <c r="F35" s="26">
         <v>44.8</v>
       </c>
-      <c r="G35" s="17">
-        <v>44.8</v>
-      </c>
-      <c r="H35" s="17">
+      <c r="G35" s="26">
         <f t="shared" si="0"/>
-        <v>44.8</v>
-      </c>
-      <c r="I35" s="26">
-        <f t="shared" si="1"/>
         <v>318.95</v>
       </c>
-      <c r="J35" s="107">
+      <c r="H35" s="107">
         <v>25</v>
       </c>
-      <c r="K35" s="116">
+      <c r="I35" s="116">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L35" s="27">
+      <c r="J35" s="27">
         <v>4.8</v>
       </c>
-      <c r="M35" s="17"/>
-      <c r="N35" s="119"/>
-      <c r="O35" s="159"/>
+      <c r="K35" s="17">
+        <v>19.8</v>
+      </c>
+      <c r="L35" s="119">
+        <v>0.19417000000000001</v>
+      </c>
+      <c r="M35" s="159"/>
+      <c r="N35" s="162"/>
+      <c r="O35" s="162"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="137"/>
@@ -6095,32 +6209,31 @@
       <c r="E36" s="111">
         <v>36</v>
       </c>
-      <c r="F36" s="27">
-        <v>44.5</v>
-      </c>
-      <c r="G36" s="17">
-        <v>44.7</v>
-      </c>
-      <c r="H36" s="17">
+      <c r="F36" s="26">
+        <v>44.6</v>
+      </c>
+      <c r="G36" s="26">
         <f t="shared" si="0"/>
-        <v>44.6</v>
-      </c>
-      <c r="I36" s="26">
-        <f t="shared" si="1"/>
         <v>318.75</v>
       </c>
-      <c r="J36" s="107">
+      <c r="H36" s="107">
         <v>25</v>
       </c>
-      <c r="K36" s="116">
+      <c r="I36" s="116">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L36" s="27">
+      <c r="J36" s="27">
         <v>8</v>
       </c>
-      <c r="M36" s="17"/>
-      <c r="N36" s="119"/>
-      <c r="O36" s="159"/>
+      <c r="K36" s="17">
+        <v>23</v>
+      </c>
+      <c r="L36" s="119">
+        <v>0.13306000000000001</v>
+      </c>
+      <c r="M36" s="159"/>
+      <c r="N36" s="162"/>
+      <c r="O36" s="162"/>
     </row>
     <row r="37" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="150"/>
@@ -6132,78 +6245,82 @@
       <c r="E37" s="113">
         <v>37</v>
       </c>
-      <c r="F37" s="29">
-        <v>45.1</v>
-      </c>
-      <c r="G37" s="18">
-        <v>44.2</v>
-      </c>
-      <c r="H37" s="18">
+      <c r="F37" s="26">
+        <v>44.650000000000006</v>
+      </c>
+      <c r="G37" s="103">
         <f t="shared" si="0"/>
-        <v>44.650000000000006</v>
-      </c>
-      <c r="I37" s="103">
-        <f t="shared" si="1"/>
         <v>318.79999999999995</v>
       </c>
-      <c r="J37" s="108">
+      <c r="H37" s="108">
         <v>25</v>
       </c>
-      <c r="K37" s="118">
+      <c r="I37" s="118">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L37" s="29">
+      <c r="J37" s="29">
         <v>12.4</v>
       </c>
-      <c r="M37" s="18"/>
-      <c r="N37" s="120"/>
-      <c r="O37" s="160"/>
+      <c r="K37" s="18">
+        <v>27.4</v>
+      </c>
+      <c r="L37" s="120">
+        <v>3.3009999999999998E-2</v>
+      </c>
+      <c r="M37" s="160"/>
+      <c r="N37" s="163"/>
+      <c r="O37" s="163"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="161">
+      <c r="A38" s="164">
         <v>8</v>
       </c>
       <c r="B38" s="122">
         <v>1</v>
       </c>
-      <c r="C38" s="162">
+      <c r="C38" s="165">
         <v>50</v>
       </c>
-      <c r="D38" s="162">
-        <f t="shared" ref="D38" si="14">C38+273.15</f>
+      <c r="D38" s="165">
+        <f t="shared" ref="D38" si="25">C38+273.15</f>
         <v>323.14999999999998</v>
       </c>
       <c r="E38" s="123">
         <v>38</v>
       </c>
-      <c r="F38" s="124">
-        <v>49.1</v>
-      </c>
-      <c r="G38" s="125">
-        <v>49.5</v>
-      </c>
-      <c r="H38" s="125">
+      <c r="F38" s="26">
+        <v>49.3</v>
+      </c>
+      <c r="G38" s="126">
         <f t="shared" si="0"/>
-        <v>49.3</v>
-      </c>
-      <c r="I38" s="126">
-        <f t="shared" si="1"/>
         <v>323.45</v>
       </c>
-      <c r="J38" s="127">
+      <c r="H38" s="127">
         <v>25</v>
       </c>
-      <c r="K38" s="128">
+      <c r="I38" s="128">
         <v>0.31</v>
       </c>
-      <c r="L38" s="124">
+      <c r="J38" s="124">
         <v>4.5999999999999996</v>
       </c>
-      <c r="M38" s="125"/>
-      <c r="N38" s="129"/>
-      <c r="O38" s="158" t="e">
-        <f t="shared" ref="O38" si="15">AVERAGE(N38:N42)</f>
-        <v>#DIV/0!</v>
+      <c r="K38" s="125">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="L38" s="129">
+        <v>0.17294999999999999</v>
+      </c>
+      <c r="M38" s="158">
+        <f t="shared" ref="M38" si="26">AVERAGE(L38:L42)</f>
+        <v>0.10080799999999998</v>
+      </c>
+      <c r="N38" s="161">
+        <f t="shared" ref="N38" si="27">O38/SQRT(5)</f>
+        <v>2.0893128391890024E-2</v>
+      </c>
+      <c r="O38" s="161">
+        <f t="shared" ref="O38" si="28">_xlfn.STDEV.S(L38:L42)</f>
+        <v>4.6718455346896962E-2</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -6216,32 +6333,31 @@
       <c r="E39" s="111">
         <v>39</v>
       </c>
-      <c r="F39" s="27">
-        <v>49.8</v>
-      </c>
-      <c r="G39" s="17">
-        <v>49</v>
-      </c>
-      <c r="H39" s="17">
+      <c r="F39" s="26">
+        <v>49.4</v>
+      </c>
+      <c r="G39" s="26">
         <f t="shared" si="0"/>
-        <v>49.4</v>
-      </c>
-      <c r="I39" s="26">
-        <f t="shared" si="1"/>
         <v>323.54999999999995</v>
       </c>
-      <c r="J39" s="107">
+      <c r="H39" s="107">
         <v>25</v>
       </c>
-      <c r="K39" s="116">
+      <c r="I39" s="116">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L39" s="27">
+      <c r="J39" s="27">
         <v>9.8000000000000007</v>
       </c>
-      <c r="M39" s="17"/>
-      <c r="N39" s="119"/>
-      <c r="O39" s="159"/>
+      <c r="K39" s="17">
+        <v>24.8</v>
+      </c>
+      <c r="L39" s="119">
+        <v>5.9319999999999998E-2</v>
+      </c>
+      <c r="M39" s="159"/>
+      <c r="N39" s="162"/>
+      <c r="O39" s="162"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="137"/>
@@ -6253,32 +6369,31 @@
       <c r="E40" s="111">
         <v>40</v>
       </c>
-      <c r="F40" s="27">
-        <v>49</v>
-      </c>
-      <c r="G40" s="17">
-        <v>48.1</v>
-      </c>
-      <c r="H40" s="17">
+      <c r="F40" s="26">
+        <v>48.55</v>
+      </c>
+      <c r="G40" s="26">
         <f t="shared" si="0"/>
-        <v>48.55</v>
-      </c>
-      <c r="I40" s="26">
-        <f t="shared" si="1"/>
         <v>322.7</v>
       </c>
-      <c r="J40" s="107">
+      <c r="H40" s="107">
         <v>25</v>
       </c>
-      <c r="K40" s="116">
+      <c r="I40" s="116">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L40" s="27">
+      <c r="J40" s="27">
         <v>11.4</v>
       </c>
-      <c r="M40" s="17"/>
-      <c r="N40" s="119"/>
-      <c r="O40" s="159"/>
+      <c r="K40" s="17">
+        <v>26.4</v>
+      </c>
+      <c r="L40" s="119">
+        <v>7.1830000000000005E-2</v>
+      </c>
+      <c r="M40" s="159"/>
+      <c r="N40" s="162"/>
+      <c r="O40" s="162"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="149"/>
@@ -6290,32 +6405,31 @@
       <c r="E41" s="112">
         <v>41</v>
       </c>
-      <c r="F41" s="27">
-        <v>49.2</v>
-      </c>
-      <c r="G41" s="17">
-        <v>49.7</v>
-      </c>
-      <c r="H41" s="17">
+      <c r="F41" s="26">
+        <v>49.45</v>
+      </c>
+      <c r="G41" s="26">
         <f t="shared" si="0"/>
-        <v>49.45</v>
-      </c>
-      <c r="I41" s="26">
-        <f t="shared" si="1"/>
         <v>323.59999999999997</v>
       </c>
-      <c r="J41" s="107">
+      <c r="H41" s="107">
         <v>25</v>
       </c>
-      <c r="K41" s="117">
+      <c r="I41" s="117">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L41" s="27">
+      <c r="J41" s="27">
         <v>5.2</v>
       </c>
-      <c r="M41" s="17"/>
-      <c r="N41" s="119"/>
-      <c r="O41" s="159"/>
+      <c r="K41" s="17">
+        <v>20.2</v>
+      </c>
+      <c r="L41" s="119">
+        <v>0.12192</v>
+      </c>
+      <c r="M41" s="159"/>
+      <c r="N41" s="162"/>
+      <c r="O41" s="162"/>
     </row>
     <row r="42" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="150"/>
@@ -6327,40 +6441,47 @@
       <c r="E42" s="113">
         <v>42</v>
       </c>
-      <c r="F42" s="29">
-        <v>49.7</v>
-      </c>
-      <c r="G42" s="18">
-        <v>49.9</v>
-      </c>
-      <c r="H42" s="18">
+      <c r="F42" s="103">
+        <v>49.8</v>
+      </c>
+      <c r="G42" s="103">
         <f t="shared" si="0"/>
-        <v>49.8</v>
-      </c>
-      <c r="I42" s="103">
-        <f t="shared" si="1"/>
         <v>323.95</v>
       </c>
-      <c r="J42" s="108">
+      <c r="H42" s="108">
         <v>25</v>
       </c>
-      <c r="K42" s="118">
+      <c r="I42" s="118">
         <v>0.28999999999999998</v>
       </c>
-      <c r="L42" s="29">
+      <c r="J42" s="29">
         <v>11.2</v>
       </c>
-      <c r="M42" s="18"/>
-      <c r="N42" s="120"/>
-      <c r="O42" s="160"/>
+      <c r="K42" s="18">
+        <v>26.2</v>
+      </c>
+      <c r="L42" s="120">
+        <v>7.8020000000000006E-2</v>
+      </c>
+      <c r="M42" s="160"/>
+      <c r="N42" s="163"/>
+      <c r="O42" s="163"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="50">
+    <mergeCell ref="O28:O32"/>
+    <mergeCell ref="O33:O37"/>
+    <mergeCell ref="O38:O42"/>
+    <mergeCell ref="O8:O12"/>
+    <mergeCell ref="O13:O17"/>
+    <mergeCell ref="O18:O22"/>
+    <mergeCell ref="O23:O27"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="D3:D7"/>
     <mergeCell ref="S3:S4"/>
+    <mergeCell ref="M3:M7"/>
     <mergeCell ref="O3:O7"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="C8:C12"/>
@@ -6383,18 +6504,26 @@
     <mergeCell ref="A33:A37"/>
     <mergeCell ref="C33:C37"/>
     <mergeCell ref="D33:D37"/>
-    <mergeCell ref="O33:O37"/>
-    <mergeCell ref="O38:O42"/>
-    <mergeCell ref="O8:O12"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="O18:O22"/>
-    <mergeCell ref="O23:O27"/>
-    <mergeCell ref="O28:O32"/>
+    <mergeCell ref="M33:M37"/>
+    <mergeCell ref="M38:M42"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="N8:N12"/>
+    <mergeCell ref="N13:N17"/>
+    <mergeCell ref="N18:N22"/>
+    <mergeCell ref="N23:N27"/>
+    <mergeCell ref="N28:N32"/>
+    <mergeCell ref="N33:N37"/>
+    <mergeCell ref="N38:N42"/>
+    <mergeCell ref="M8:M12"/>
+    <mergeCell ref="M13:M17"/>
+    <mergeCell ref="M18:M22"/>
+    <mergeCell ref="M23:M27"/>
+    <mergeCell ref="M28:M32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H3:H42" formulaRange="1"/>
+    <ignoredError sqref="M3:M42 O3:O42" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6495,351 +6624,351 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" ht="25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="177" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="175"/>
-      <c r="C1" s="175"/>
-      <c r="D1" s="175"/>
-      <c r="E1" s="175"/>
-      <c r="F1" s="175"/>
-      <c r="G1" s="175"/>
-      <c r="H1" s="175"/>
-      <c r="I1" s="175"/>
-      <c r="J1" s="175"/>
-      <c r="K1" s="175"/>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
-      <c r="O1" s="175"/>
-      <c r="P1" s="175"/>
-      <c r="Q1" s="175"/>
-      <c r="R1" s="175"/>
-      <c r="S1" s="175"/>
-      <c r="T1" s="175"/>
-      <c r="U1" s="175"/>
-      <c r="V1" s="175"/>
-      <c r="W1" s="175"/>
-      <c r="X1" s="175"/>
-      <c r="Y1" s="175"/>
-      <c r="Z1" s="175"/>
-      <c r="AA1" s="175"/>
-      <c r="AB1" s="175"/>
-      <c r="AC1" s="175"/>
-      <c r="AD1" s="175"/>
-      <c r="AE1" s="175"/>
-      <c r="AF1" s="175"/>
-      <c r="AG1" s="175"/>
-      <c r="AH1" s="175"/>
-      <c r="AI1" s="175"/>
-      <c r="AJ1" s="175"/>
-      <c r="AK1" s="175"/>
-      <c r="AL1" s="175"/>
-      <c r="AM1" s="175"/>
-      <c r="AN1" s="175"/>
-      <c r="AO1" s="175"/>
-      <c r="AP1" s="175"/>
-      <c r="AQ1" s="175"/>
-      <c r="AR1" s="175"/>
-      <c r="AS1" s="175"/>
-      <c r="AT1" s="175"/>
-      <c r="AU1" s="175"/>
-      <c r="AV1" s="175"/>
-      <c r="AW1" s="175"/>
-      <c r="AX1" s="175"/>
-      <c r="AY1" s="175"/>
-      <c r="AZ1" s="175"/>
-      <c r="BA1" s="175"/>
-      <c r="BB1" s="175"/>
-      <c r="BC1" s="175"/>
-      <c r="BD1" s="175"/>
-      <c r="BE1" s="175"/>
-      <c r="BF1" s="175"/>
-      <c r="BG1" s="175"/>
-      <c r="BH1" s="175"/>
-      <c r="BI1" s="175"/>
-      <c r="BJ1" s="175"/>
-      <c r="BK1" s="175"/>
-      <c r="BL1" s="175"/>
-      <c r="BM1" s="175"/>
-      <c r="BN1" s="175"/>
-      <c r="BO1" s="175"/>
-      <c r="BP1" s="175"/>
-      <c r="BQ1" s="175"/>
-      <c r="BR1" s="175"/>
-      <c r="BS1" s="175"/>
-      <c r="BT1" s="175"/>
-      <c r="BU1" s="175"/>
-      <c r="BV1" s="175"/>
-      <c r="BW1" s="175"/>
-      <c r="BX1" s="175"/>
-      <c r="BY1" s="175"/>
-      <c r="BZ1" s="175"/>
-      <c r="CA1" s="175"/>
-      <c r="CB1" s="175"/>
-      <c r="CC1" s="176"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+      <c r="M1" s="178"/>
+      <c r="N1" s="178"/>
+      <c r="O1" s="178"/>
+      <c r="P1" s="178"/>
+      <c r="Q1" s="178"/>
+      <c r="R1" s="178"/>
+      <c r="S1" s="178"/>
+      <c r="T1" s="178"/>
+      <c r="U1" s="178"/>
+      <c r="V1" s="178"/>
+      <c r="W1" s="178"/>
+      <c r="X1" s="178"/>
+      <c r="Y1" s="178"/>
+      <c r="Z1" s="178"/>
+      <c r="AA1" s="178"/>
+      <c r="AB1" s="178"/>
+      <c r="AC1" s="178"/>
+      <c r="AD1" s="178"/>
+      <c r="AE1" s="178"/>
+      <c r="AF1" s="178"/>
+      <c r="AG1" s="178"/>
+      <c r="AH1" s="178"/>
+      <c r="AI1" s="178"/>
+      <c r="AJ1" s="178"/>
+      <c r="AK1" s="178"/>
+      <c r="AL1" s="178"/>
+      <c r="AM1" s="178"/>
+      <c r="AN1" s="178"/>
+      <c r="AO1" s="178"/>
+      <c r="AP1" s="178"/>
+      <c r="AQ1" s="178"/>
+      <c r="AR1" s="178"/>
+      <c r="AS1" s="178"/>
+      <c r="AT1" s="178"/>
+      <c r="AU1" s="178"/>
+      <c r="AV1" s="178"/>
+      <c r="AW1" s="178"/>
+      <c r="AX1" s="178"/>
+      <c r="AY1" s="178"/>
+      <c r="AZ1" s="178"/>
+      <c r="BA1" s="178"/>
+      <c r="BB1" s="178"/>
+      <c r="BC1" s="178"/>
+      <c r="BD1" s="178"/>
+      <c r="BE1" s="178"/>
+      <c r="BF1" s="178"/>
+      <c r="BG1" s="178"/>
+      <c r="BH1" s="178"/>
+      <c r="BI1" s="178"/>
+      <c r="BJ1" s="178"/>
+      <c r="BK1" s="178"/>
+      <c r="BL1" s="178"/>
+      <c r="BM1" s="178"/>
+      <c r="BN1" s="178"/>
+      <c r="BO1" s="178"/>
+      <c r="BP1" s="178"/>
+      <c r="BQ1" s="178"/>
+      <c r="BR1" s="178"/>
+      <c r="BS1" s="178"/>
+      <c r="BT1" s="178"/>
+      <c r="BU1" s="178"/>
+      <c r="BV1" s="178"/>
+      <c r="BW1" s="178"/>
+      <c r="BX1" s="178"/>
+      <c r="BY1" s="178"/>
+      <c r="BZ1" s="178"/>
+      <c r="CA1" s="178"/>
+      <c r="CB1" s="178"/>
+      <c r="CC1" s="179"/>
     </row>
     <row r="2" spans="1:81" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="167"/>
-      <c r="B2" s="177" t="s">
+      <c r="A2" s="170"/>
+      <c r="B2" s="180" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="178"/>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
-      <c r="I2" s="178"/>
-      <c r="J2" s="178"/>
-      <c r="K2" s="178"/>
-      <c r="L2" s="178" t="s">
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="181"/>
+      <c r="H2" s="181"/>
+      <c r="I2" s="181"/>
+      <c r="J2" s="181"/>
+      <c r="K2" s="181"/>
+      <c r="L2" s="181" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="178"/>
-      <c r="N2" s="178"/>
-      <c r="O2" s="178"/>
-      <c r="P2" s="178"/>
-      <c r="Q2" s="178"/>
-      <c r="R2" s="178"/>
-      <c r="S2" s="178"/>
-      <c r="T2" s="178"/>
-      <c r="U2" s="178"/>
-      <c r="V2" s="178" t="s">
+      <c r="M2" s="181"/>
+      <c r="N2" s="181"/>
+      <c r="O2" s="181"/>
+      <c r="P2" s="181"/>
+      <c r="Q2" s="181"/>
+      <c r="R2" s="181"/>
+      <c r="S2" s="181"/>
+      <c r="T2" s="181"/>
+      <c r="U2" s="181"/>
+      <c r="V2" s="181" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="178"/>
-      <c r="X2" s="178"/>
-      <c r="Y2" s="178"/>
-      <c r="Z2" s="178"/>
-      <c r="AA2" s="178"/>
-      <c r="AB2" s="178"/>
-      <c r="AC2" s="178"/>
-      <c r="AD2" s="178"/>
-      <c r="AE2" s="178"/>
-      <c r="AF2" s="178" t="s">
+      <c r="W2" s="181"/>
+      <c r="X2" s="181"/>
+      <c r="Y2" s="181"/>
+      <c r="Z2" s="181"/>
+      <c r="AA2" s="181"/>
+      <c r="AB2" s="181"/>
+      <c r="AC2" s="181"/>
+      <c r="AD2" s="181"/>
+      <c r="AE2" s="181"/>
+      <c r="AF2" s="181" t="s">
         <v>40</v>
       </c>
-      <c r="AG2" s="178"/>
-      <c r="AH2" s="178"/>
-      <c r="AI2" s="178"/>
-      <c r="AJ2" s="178"/>
-      <c r="AK2" s="178"/>
-      <c r="AL2" s="178"/>
-      <c r="AM2" s="178"/>
-      <c r="AN2" s="178"/>
-      <c r="AO2" s="178"/>
-      <c r="AP2" s="178" t="s">
+      <c r="AG2" s="181"/>
+      <c r="AH2" s="181"/>
+      <c r="AI2" s="181"/>
+      <c r="AJ2" s="181"/>
+      <c r="AK2" s="181"/>
+      <c r="AL2" s="181"/>
+      <c r="AM2" s="181"/>
+      <c r="AN2" s="181"/>
+      <c r="AO2" s="181"/>
+      <c r="AP2" s="181" t="s">
         <v>41</v>
       </c>
-      <c r="AQ2" s="178"/>
-      <c r="AR2" s="178"/>
-      <c r="AS2" s="178"/>
-      <c r="AT2" s="178"/>
-      <c r="AU2" s="178"/>
-      <c r="AV2" s="178"/>
-      <c r="AW2" s="178"/>
-      <c r="AX2" s="178"/>
-      <c r="AY2" s="178"/>
-      <c r="AZ2" s="178" t="s">
+      <c r="AQ2" s="181"/>
+      <c r="AR2" s="181"/>
+      <c r="AS2" s="181"/>
+      <c r="AT2" s="181"/>
+      <c r="AU2" s="181"/>
+      <c r="AV2" s="181"/>
+      <c r="AW2" s="181"/>
+      <c r="AX2" s="181"/>
+      <c r="AY2" s="181"/>
+      <c r="AZ2" s="181" t="s">
         <v>42</v>
       </c>
-      <c r="BA2" s="178"/>
-      <c r="BB2" s="178"/>
-      <c r="BC2" s="178"/>
-      <c r="BD2" s="178"/>
-      <c r="BE2" s="178"/>
-      <c r="BF2" s="178"/>
-      <c r="BG2" s="178"/>
-      <c r="BH2" s="178"/>
-      <c r="BI2" s="178"/>
-      <c r="BJ2" s="178" t="s">
+      <c r="BA2" s="181"/>
+      <c r="BB2" s="181"/>
+      <c r="BC2" s="181"/>
+      <c r="BD2" s="181"/>
+      <c r="BE2" s="181"/>
+      <c r="BF2" s="181"/>
+      <c r="BG2" s="181"/>
+      <c r="BH2" s="181"/>
+      <c r="BI2" s="181"/>
+      <c r="BJ2" s="181" t="s">
         <v>43</v>
       </c>
-      <c r="BK2" s="178"/>
-      <c r="BL2" s="178"/>
-      <c r="BM2" s="178"/>
-      <c r="BN2" s="178"/>
-      <c r="BO2" s="178"/>
-      <c r="BP2" s="178"/>
-      <c r="BQ2" s="178"/>
-      <c r="BR2" s="178"/>
-      <c r="BS2" s="178"/>
-      <c r="BT2" s="178" t="s">
+      <c r="BK2" s="181"/>
+      <c r="BL2" s="181"/>
+      <c r="BM2" s="181"/>
+      <c r="BN2" s="181"/>
+      <c r="BO2" s="181"/>
+      <c r="BP2" s="181"/>
+      <c r="BQ2" s="181"/>
+      <c r="BR2" s="181"/>
+      <c r="BS2" s="181"/>
+      <c r="BT2" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="BU2" s="178"/>
-      <c r="BV2" s="178"/>
-      <c r="BW2" s="178"/>
-      <c r="BX2" s="178"/>
-      <c r="BY2" s="178"/>
-      <c r="BZ2" s="178"/>
-      <c r="CA2" s="178"/>
-      <c r="CB2" s="178"/>
-      <c r="CC2" s="179"/>
+      <c r="BU2" s="181"/>
+      <c r="BV2" s="181"/>
+      <c r="BW2" s="181"/>
+      <c r="BX2" s="181"/>
+      <c r="BY2" s="181"/>
+      <c r="BZ2" s="181"/>
+      <c r="CA2" s="181"/>
+      <c r="CB2" s="181"/>
+      <c r="CC2" s="182"/>
     </row>
     <row r="3" spans="1:81" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="168"/>
-      <c r="B3" s="165" t="s">
+      <c r="A3" s="171"/>
+      <c r="B3" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="166"/>
-      <c r="D3" s="169" t="s">
+      <c r="C3" s="169"/>
+      <c r="D3" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="170"/>
-      <c r="F3" s="169" t="s">
+      <c r="E3" s="173"/>
+      <c r="F3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="170"/>
-      <c r="H3" s="169" t="s">
+      <c r="G3" s="173"/>
+      <c r="H3" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="170"/>
-      <c r="J3" s="171" t="s">
+      <c r="I3" s="173"/>
+      <c r="J3" s="174" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="172"/>
-      <c r="L3" s="169" t="s">
+      <c r="K3" s="175"/>
+      <c r="L3" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="170"/>
-      <c r="N3" s="169" t="s">
+      <c r="M3" s="173"/>
+      <c r="N3" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="170"/>
-      <c r="P3" s="169" t="s">
+      <c r="O3" s="173"/>
+      <c r="P3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="170"/>
-      <c r="R3" s="169" t="s">
+      <c r="Q3" s="173"/>
+      <c r="R3" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="170"/>
-      <c r="T3" s="169" t="s">
+      <c r="S3" s="173"/>
+      <c r="T3" s="172" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="170"/>
-      <c r="V3" s="169" t="s">
+      <c r="U3" s="173"/>
+      <c r="V3" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="W3" s="170"/>
-      <c r="X3" s="169" t="s">
+      <c r="W3" s="173"/>
+      <c r="X3" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="170"/>
-      <c r="Z3" s="169" t="s">
+      <c r="Y3" s="173"/>
+      <c r="Z3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="AA3" s="170"/>
-      <c r="AB3" s="169" t="s">
+      <c r="AA3" s="173"/>
+      <c r="AB3" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="170"/>
-      <c r="AD3" s="169" t="s">
+      <c r="AC3" s="173"/>
+      <c r="AD3" s="172" t="s">
         <v>33</v>
       </c>
-      <c r="AE3" s="170"/>
-      <c r="AF3" s="169" t="s">
+      <c r="AE3" s="173"/>
+      <c r="AF3" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="AG3" s="170"/>
-      <c r="AH3" s="169" t="s">
+      <c r="AG3" s="173"/>
+      <c r="AH3" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="AI3" s="170"/>
-      <c r="AJ3" s="169" t="s">
+      <c r="AI3" s="173"/>
+      <c r="AJ3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="AK3" s="170"/>
-      <c r="AL3" s="169" t="s">
+      <c r="AK3" s="173"/>
+      <c r="AL3" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="AM3" s="170"/>
-      <c r="AN3" s="169" t="s">
+      <c r="AM3" s="173"/>
+      <c r="AN3" s="172" t="s">
         <v>33</v>
       </c>
-      <c r="AO3" s="170"/>
-      <c r="AP3" s="169" t="s">
+      <c r="AO3" s="173"/>
+      <c r="AP3" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="170"/>
-      <c r="AR3" s="169" t="s">
+      <c r="AQ3" s="173"/>
+      <c r="AR3" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="AS3" s="170"/>
-      <c r="AT3" s="169" t="s">
+      <c r="AS3" s="173"/>
+      <c r="AT3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="AU3" s="170"/>
-      <c r="AV3" s="169" t="s">
+      <c r="AU3" s="173"/>
+      <c r="AV3" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="AW3" s="170"/>
-      <c r="AX3" s="169" t="s">
+      <c r="AW3" s="173"/>
+      <c r="AX3" s="172" t="s">
         <v>33</v>
       </c>
-      <c r="AY3" s="170"/>
-      <c r="AZ3" s="169" t="s">
+      <c r="AY3" s="173"/>
+      <c r="AZ3" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="BA3" s="170"/>
-      <c r="BB3" s="169" t="s">
+      <c r="BA3" s="173"/>
+      <c r="BB3" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="BC3" s="170"/>
-      <c r="BD3" s="169" t="s">
+      <c r="BC3" s="173"/>
+      <c r="BD3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="BE3" s="170"/>
-      <c r="BF3" s="169" t="s">
+      <c r="BE3" s="173"/>
+      <c r="BF3" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="BG3" s="170"/>
-      <c r="BH3" s="169" t="s">
+      <c r="BG3" s="173"/>
+      <c r="BH3" s="172" t="s">
         <v>33</v>
       </c>
-      <c r="BI3" s="170"/>
-      <c r="BJ3" s="169" t="s">
+      <c r="BI3" s="173"/>
+      <c r="BJ3" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="BK3" s="170"/>
-      <c r="BL3" s="169" t="s">
+      <c r="BK3" s="173"/>
+      <c r="BL3" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="BM3" s="170"/>
-      <c r="BN3" s="169" t="s">
+      <c r="BM3" s="173"/>
+      <c r="BN3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="BO3" s="170"/>
-      <c r="BP3" s="169" t="s">
+      <c r="BO3" s="173"/>
+      <c r="BP3" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="BQ3" s="170"/>
-      <c r="BR3" s="173" t="s">
+      <c r="BQ3" s="173"/>
+      <c r="BR3" s="176" t="s">
         <v>33</v>
       </c>
-      <c r="BS3" s="166"/>
-      <c r="BT3" s="169" t="s">
+      <c r="BS3" s="169"/>
+      <c r="BT3" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="BU3" s="170"/>
-      <c r="BV3" s="169" t="s">
+      <c r="BU3" s="173"/>
+      <c r="BV3" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="BW3" s="170"/>
-      <c r="BX3" s="169" t="s">
+      <c r="BW3" s="173"/>
+      <c r="BX3" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="BY3" s="170"/>
-      <c r="BZ3" s="169" t="s">
+      <c r="BY3" s="173"/>
+      <c r="BZ3" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="CA3" s="170"/>
-      <c r="CB3" s="169" t="s">
+      <c r="CA3" s="173"/>
+      <c r="CB3" s="172" t="s">
         <v>33</v>
       </c>
-      <c r="CC3" s="170"/>
+      <c r="CC3" s="173"/>
     </row>
     <row r="4" spans="1:81" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">

</xml_diff>

<commit_message>
Update report with new title and enhanced data processing details. Modify HTML structure in `interactive_pressure_analysis.py` to reflect the new focus on "Chemistry IA Data." Revise LaTeX document to include additional steps for uncertainty propagation and data analysis, along with updated table structures and bookmarks for improved navigation.
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wrca-my.sharepoint.com/personal/huj26_mywrca_ca/Documents/12/Chemistry HL/Chemistry IA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1772" documentId="8_{ED69E5BD-9A97-5849-9651-1A764BC4410F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC7D8A26-372A-B54C-AB12-C1D4ADB4920F}"/>
+  <xr:revisionPtr revIDLastSave="1781" documentId="8_{ED69E5BD-9A97-5849-9651-1A764BC4410F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05FDAB0B-4D7F-B64C-9457-289D613BAFB2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{3196E468-6A35-EA40-9409-42F714E37880}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{3196E468-6A35-EA40-9409-42F714E37880}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="56">
   <si>
     <t>Target (°C)</t>
   </si>
@@ -375,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1018,17 +1018,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1050,21 +1039,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1110,7 +1084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1436,25 +1410,16 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="6" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1478,9 +1443,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1490,34 +1452,16 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="11" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1604,9 +1548,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1656,6 +1597,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1759,9 +1703,9 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="44450" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1831,7 +1775,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Processed Data'!$O$3:$O$42</c:f>
+                <c:f>'Processed Data'!$M$3:$M$42</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="40"/>
@@ -1864,7 +1808,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Processed Data'!$O$3:$O$42</c:f>
+                <c:f>'Processed Data'!$M$3:$M$42</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="40"/>
@@ -1944,33 +1888,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Processed Data'!$O$3:$O$42</c:f>
+              <c:f>'Processed Data'!$L$3:$L$42</c:f>
               <c:numCache>
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>4.336020064529226E-3</c:v>
+                  <c:v>1.9391271232180748E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9758788168523553E-3</c:v>
+                  <c:v>2.2252806564566183E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.0545694411494834E-3</c:v>
+                  <c:v>3.1548993644805894E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.9442640509971881E-2</c:v>
+                  <c:v>8.6950131684776603E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.3418992883223374E-2</c:v>
+                  <c:v>6.0011560552946722E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.847383338671214E-2</c:v>
+                  <c:v>8.2617494515387011E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.8257707623388592E-2</c:v>
+                  <c:v>3.0525774846840499E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.6718455346896962E-2</c:v>
+                  <c:v>2.0893128391890024E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2850,13 +2794,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>8912</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>155964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>534736</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -3206,8 +3150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFD131A-068C-8045-AE76-58186661ABFD}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I42"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3237,29 +3181,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="147"/>
-      <c r="M1" s="147"/>
-      <c r="N1" s="147"/>
-      <c r="O1" s="148"/>
-      <c r="Q1" s="141" t="s">
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="137"/>
+      <c r="O1" s="138"/>
+      <c r="Q1" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="142"/>
-      <c r="S1" s="142"/>
-      <c r="T1" s="143"/>
+      <c r="R1" s="132"/>
+      <c r="S1" s="132"/>
+      <c r="T1" s="133"/>
     </row>
     <row r="2" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3321,23 +3265,23 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="140">
+      <c r="A3" s="130">
         <v>1</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="139">
+      <c r="C3" s="129">
         <v>15</v>
       </c>
-      <c r="D3" s="139">
+      <c r="D3" s="129">
         <f>C3+273.15</f>
         <v>288.14999999999998</v>
       </c>
       <c r="E3" s="21">
         <v>4</v>
       </c>
-      <c r="F3" s="157">
+      <c r="F3" s="147">
         <v>45</v>
       </c>
       <c r="G3" s="25">
@@ -3366,22 +3310,22 @@
       <c r="R3" s="44">
         <v>5</v>
       </c>
-      <c r="S3" s="151" t="s">
+      <c r="S3" s="141" t="s">
         <v>45</v>
       </c>
       <c r="T3" s="14"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="137"/>
+      <c r="A4" s="127"/>
       <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
       <c r="E4" s="22">
         <v>5</v>
       </c>
-      <c r="F4" s="154"/>
+      <c r="F4" s="144"/>
       <c r="G4" s="27">
         <v>15.4</v>
       </c>
@@ -3408,20 +3352,20 @@
       <c r="R4" s="10">
         <v>60</v>
       </c>
-      <c r="S4" s="152"/>
+      <c r="S4" s="142"/>
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="137"/>
+      <c r="A5" s="127"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
       <c r="E5" s="22">
         <v>6</v>
       </c>
-      <c r="F5" s="154"/>
+      <c r="F5" s="144"/>
       <c r="G5" s="27">
         <v>14.7</v>
       </c>
@@ -3454,16 +3398,16 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="137"/>
+      <c r="A6" s="127"/>
       <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="138"/>
-      <c r="D6" s="138"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
       <c r="E6" s="22">
         <v>7</v>
       </c>
-      <c r="F6" s="154"/>
+      <c r="F6" s="144"/>
       <c r="G6" s="27">
         <v>14.9</v>
       </c>
@@ -3496,16 +3440,16 @@
       <c r="T6" s="15"/>
     </row>
     <row r="7" spans="1:20" ht="68" x14ac:dyDescent="0.2">
-      <c r="A7" s="137"/>
+      <c r="A7" s="127"/>
       <c r="B7" s="91">
         <v>5</v>
       </c>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
       <c r="E7" s="90">
         <v>8</v>
       </c>
-      <c r="F7" s="155"/>
+      <c r="F7" s="145"/>
       <c r="G7" s="92">
         <v>15.32</v>
       </c>
@@ -3540,23 +3484,23 @@
       <c r="T7" s="15"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="137">
+      <c r="A8" s="127">
         <v>2</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="138">
+      <c r="C8" s="128">
         <v>20</v>
       </c>
-      <c r="D8" s="138">
+      <c r="D8" s="128">
         <f t="shared" ref="D8" si="1">C8+273.15</f>
         <v>293.14999999999998</v>
       </c>
       <c r="E8" s="22">
         <v>48</v>
       </c>
-      <c r="F8" s="153">
+      <c r="F8" s="143">
         <v>55</v>
       </c>
       <c r="G8" s="27">
@@ -3591,16 +3535,16 @@
       <c r="T8" s="15"/>
     </row>
     <row r="9" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="137"/>
+      <c r="A9" s="127"/>
       <c r="B9" s="7">
         <v>2</v>
       </c>
-      <c r="C9" s="138"/>
-      <c r="D9" s="138"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="128"/>
       <c r="E9" s="22">
         <v>9</v>
       </c>
-      <c r="F9" s="154"/>
+      <c r="F9" s="144"/>
       <c r="G9" s="27">
         <v>21.4</v>
       </c>
@@ -3633,16 +3577,16 @@
       <c r="T9" s="16"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="137"/>
+      <c r="A10" s="127"/>
       <c r="B10" s="7">
         <v>3</v>
       </c>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
       <c r="E10" s="22">
         <v>10</v>
       </c>
-      <c r="F10" s="154"/>
+      <c r="F10" s="144"/>
       <c r="G10" s="27">
         <v>21</v>
       </c>
@@ -3665,16 +3609,16 @@
       <c r="O10" s="98"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="137"/>
+      <c r="A11" s="127"/>
       <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
       <c r="E11" s="22">
         <v>11</v>
       </c>
-      <c r="F11" s="154"/>
+      <c r="F11" s="144"/>
       <c r="G11" s="27">
         <v>19.7</v>
       </c>
@@ -3697,16 +3641,16 @@
       <c r="O11" s="98"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="137"/>
+      <c r="A12" s="127"/>
       <c r="B12" s="7">
         <v>5</v>
       </c>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="128"/>
       <c r="E12" s="22">
         <v>12</v>
       </c>
-      <c r="F12" s="155"/>
+      <c r="F12" s="145"/>
       <c r="G12" s="27">
         <v>19.3</v>
       </c>
@@ -3729,23 +3673,23 @@
       <c r="O12" s="98"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="137">
+      <c r="A13" s="127">
         <v>3</v>
       </c>
       <c r="B13" s="7">
         <v>1</v>
       </c>
-      <c r="C13" s="138">
+      <c r="C13" s="128">
         <v>25</v>
       </c>
-      <c r="D13" s="138">
+      <c r="D13" s="128">
         <f t="shared" ref="D13" si="2">C13+273.15</f>
         <v>298.14999999999998</v>
       </c>
       <c r="E13" s="22">
         <v>13</v>
       </c>
-      <c r="F13" s="153">
+      <c r="F13" s="143">
         <v>65</v>
       </c>
       <c r="G13" s="27">
@@ -3770,16 +3714,16 @@
       <c r="O13" s="98"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="137"/>
+      <c r="A14" s="127"/>
       <c r="B14" s="7">
         <v>2</v>
       </c>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="128"/>
       <c r="E14" s="22">
         <v>14</v>
       </c>
-      <c r="F14" s="154"/>
+      <c r="F14" s="144"/>
       <c r="G14" s="27">
         <v>25.3</v>
       </c>
@@ -3802,16 +3746,16 @@
       <c r="O14" s="98"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="137"/>
+      <c r="A15" s="127"/>
       <c r="B15" s="7">
         <v>3</v>
       </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="128"/>
       <c r="E15" s="22">
         <v>15</v>
       </c>
-      <c r="F15" s="154"/>
+      <c r="F15" s="144"/>
       <c r="G15" s="27">
         <v>25.7</v>
       </c>
@@ -3834,16 +3778,16 @@
       <c r="O15" s="98"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="137"/>
+      <c r="A16" s="127"/>
       <c r="B16" s="7">
         <v>4</v>
       </c>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="128"/>
       <c r="E16" s="22">
         <v>16</v>
       </c>
-      <c r="F16" s="154"/>
+      <c r="F16" s="144"/>
       <c r="G16" s="27">
         <v>24.7</v>
       </c>
@@ -3866,16 +3810,16 @@
       <c r="O16" s="98"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="137"/>
+      <c r="A17" s="127"/>
       <c r="B17" s="7">
         <v>5</v>
       </c>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
       <c r="E17" s="22">
         <v>17</v>
       </c>
-      <c r="F17" s="155"/>
+      <c r="F17" s="145"/>
       <c r="G17" s="27">
         <v>25.4</v>
       </c>
@@ -3898,23 +3842,23 @@
       <c r="O17" s="98"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="137">
+      <c r="A18" s="127">
         <v>4</v>
       </c>
       <c r="B18" s="7">
         <v>1</v>
       </c>
-      <c r="C18" s="138">
+      <c r="C18" s="128">
         <v>30</v>
       </c>
-      <c r="D18" s="138">
+      <c r="D18" s="128">
         <f t="shared" ref="D18" si="3">C18+273.15</f>
         <v>303.14999999999998</v>
       </c>
       <c r="E18" s="22">
         <v>18</v>
       </c>
-      <c r="F18" s="153">
+      <c r="F18" s="143">
         <v>85</v>
       </c>
       <c r="G18" s="27">
@@ -3939,16 +3883,16 @@
       <c r="O18" s="98"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="137"/>
+      <c r="A19" s="127"/>
       <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
+      <c r="C19" s="128"/>
+      <c r="D19" s="128"/>
       <c r="E19" s="22">
         <v>19</v>
       </c>
-      <c r="F19" s="154"/>
+      <c r="F19" s="144"/>
       <c r="G19" s="27">
         <v>29.1</v>
       </c>
@@ -3971,16 +3915,16 @@
       <c r="O19" s="98"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="137"/>
+      <c r="A20" s="127"/>
       <c r="B20" s="7">
         <v>3</v>
       </c>
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
+      <c r="C20" s="128"/>
+      <c r="D20" s="128"/>
       <c r="E20" s="22">
         <v>20</v>
       </c>
-      <c r="F20" s="154"/>
+      <c r="F20" s="144"/>
       <c r="G20" s="27">
         <v>30.9</v>
       </c>
@@ -4003,16 +3947,16 @@
       <c r="O20" s="98"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="137"/>
+      <c r="A21" s="127"/>
       <c r="B21" s="7">
         <v>4</v>
       </c>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
+      <c r="C21" s="128"/>
+      <c r="D21" s="128"/>
       <c r="E21" s="22">
         <v>21</v>
       </c>
-      <c r="F21" s="154"/>
+      <c r="F21" s="144"/>
       <c r="G21" s="27">
         <v>30</v>
       </c>
@@ -4035,16 +3979,16 @@
       <c r="O21" s="98"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="137"/>
+      <c r="A22" s="127"/>
       <c r="B22" s="7">
         <v>5</v>
       </c>
-      <c r="C22" s="138"/>
-      <c r="D22" s="138"/>
+      <c r="C22" s="128"/>
+      <c r="D22" s="128"/>
       <c r="E22" s="22">
         <v>22</v>
       </c>
-      <c r="F22" s="155"/>
+      <c r="F22" s="145"/>
       <c r="G22" s="27">
         <v>30.8</v>
       </c>
@@ -4067,23 +4011,23 @@
       <c r="O22" s="98"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="137">
+      <c r="A23" s="127">
         <v>5</v>
       </c>
       <c r="B23" s="7">
         <v>1</v>
       </c>
-      <c r="C23" s="138">
+      <c r="C23" s="128">
         <v>35</v>
       </c>
-      <c r="D23" s="138">
+      <c r="D23" s="128">
         <f t="shared" ref="D23" si="4">C23+273.15</f>
         <v>308.14999999999998</v>
       </c>
       <c r="E23" s="22">
         <v>23</v>
       </c>
-      <c r="F23" s="153">
+      <c r="F23" s="143">
         <v>100</v>
       </c>
       <c r="G23" s="27">
@@ -4108,16 +4052,16 @@
       <c r="O23" s="98"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="137"/>
+      <c r="A24" s="127"/>
       <c r="B24" s="7">
         <v>2</v>
       </c>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="128"/>
       <c r="E24" s="22">
         <v>24</v>
       </c>
-      <c r="F24" s="154"/>
+      <c r="F24" s="144"/>
       <c r="G24" s="27">
         <v>35.299999999999997</v>
       </c>
@@ -4140,16 +4084,16 @@
       <c r="O24" s="98"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="137"/>
+      <c r="A25" s="127"/>
       <c r="B25" s="7">
         <v>3</v>
       </c>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
+      <c r="C25" s="128"/>
+      <c r="D25" s="128"/>
       <c r="E25" s="22">
         <v>25</v>
       </c>
-      <c r="F25" s="154"/>
+      <c r="F25" s="144"/>
       <c r="G25" s="27">
         <v>35.1</v>
       </c>
@@ -4172,16 +4116,16 @@
       <c r="O25" s="98"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="137"/>
+      <c r="A26" s="127"/>
       <c r="B26" s="7">
         <v>4</v>
       </c>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
       <c r="E26" s="22">
         <v>26</v>
       </c>
-      <c r="F26" s="154"/>
+      <c r="F26" s="144"/>
       <c r="G26" s="27">
         <v>34.700000000000003</v>
       </c>
@@ -4204,16 +4148,16 @@
       <c r="O26" s="98"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="137"/>
+      <c r="A27" s="127"/>
       <c r="B27" s="7">
         <v>5</v>
       </c>
-      <c r="C27" s="138"/>
-      <c r="D27" s="138"/>
+      <c r="C27" s="128"/>
+      <c r="D27" s="128"/>
       <c r="E27" s="22">
         <v>27</v>
       </c>
-      <c r="F27" s="155"/>
+      <c r="F27" s="145"/>
       <c r="G27" s="27">
         <v>35.5</v>
       </c>
@@ -4236,23 +4180,23 @@
       <c r="O27" s="98"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="137">
+      <c r="A28" s="127">
         <v>6</v>
       </c>
       <c r="B28" s="7">
         <v>1</v>
       </c>
-      <c r="C28" s="138">
+      <c r="C28" s="128">
         <v>40</v>
       </c>
-      <c r="D28" s="138">
+      <c r="D28" s="128">
         <f t="shared" ref="D28" si="5">C28+273.15</f>
         <v>313.14999999999998</v>
       </c>
       <c r="E28" s="22">
         <v>43</v>
       </c>
-      <c r="F28" s="153">
+      <c r="F28" s="143">
         <v>125</v>
       </c>
       <c r="G28" s="27">
@@ -4277,16 +4221,16 @@
       <c r="O28" s="98"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="137"/>
+      <c r="A29" s="127"/>
       <c r="B29" s="7">
         <v>2</v>
       </c>
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
+      <c r="C29" s="128"/>
+      <c r="D29" s="128"/>
       <c r="E29" s="22">
         <v>44</v>
       </c>
-      <c r="F29" s="154"/>
+      <c r="F29" s="144"/>
       <c r="G29" s="27">
         <v>41.3</v>
       </c>
@@ -4309,16 +4253,16 @@
       <c r="O29" s="98"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="137"/>
+      <c r="A30" s="127"/>
       <c r="B30" s="7">
         <v>3</v>
       </c>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
+      <c r="C30" s="128"/>
+      <c r="D30" s="128"/>
       <c r="E30" s="22">
         <v>45</v>
       </c>
-      <c r="F30" s="154"/>
+      <c r="F30" s="144"/>
       <c r="G30" s="27">
         <v>40.5</v>
       </c>
@@ -4341,16 +4285,16 @@
       <c r="O30" s="98"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="137"/>
+      <c r="A31" s="127"/>
       <c r="B31" s="7">
         <v>4</v>
       </c>
-      <c r="C31" s="138"/>
-      <c r="D31" s="138"/>
+      <c r="C31" s="128"/>
+      <c r="D31" s="128"/>
       <c r="E31" s="22">
         <v>46</v>
       </c>
-      <c r="F31" s="154"/>
+      <c r="F31" s="144"/>
       <c r="G31" s="27">
         <v>40</v>
       </c>
@@ -4373,16 +4317,16 @@
       <c r="O31" s="98"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="137"/>
+      <c r="A32" s="127"/>
       <c r="B32" s="7">
         <v>5</v>
       </c>
-      <c r="C32" s="138"/>
-      <c r="D32" s="138"/>
+      <c r="C32" s="128"/>
+      <c r="D32" s="128"/>
       <c r="E32" s="22">
         <v>47</v>
       </c>
-      <c r="F32" s="155"/>
+      <c r="F32" s="145"/>
       <c r="G32" s="27">
         <v>39.1</v>
       </c>
@@ -4405,23 +4349,23 @@
       <c r="O32" s="98"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="137">
+      <c r="A33" s="127">
         <v>7</v>
       </c>
       <c r="B33" s="7">
         <v>1</v>
       </c>
-      <c r="C33" s="138">
+      <c r="C33" s="128">
         <v>45</v>
       </c>
-      <c r="D33" s="138">
+      <c r="D33" s="128">
         <f t="shared" ref="D33" si="6">C33+273.15</f>
         <v>318.14999999999998</v>
       </c>
       <c r="E33" s="22">
         <v>33</v>
       </c>
-      <c r="F33" s="153">
+      <c r="F33" s="143">
         <v>160</v>
       </c>
       <c r="G33" s="27">
@@ -4446,16 +4390,16 @@
       <c r="O33" s="98"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="137"/>
+      <c r="A34" s="127"/>
       <c r="B34" s="7">
         <v>2</v>
       </c>
-      <c r="C34" s="138"/>
-      <c r="D34" s="138"/>
+      <c r="C34" s="128"/>
+      <c r="D34" s="128"/>
       <c r="E34" s="22">
         <v>34</v>
       </c>
-      <c r="F34" s="154"/>
+      <c r="F34" s="144"/>
       <c r="G34" s="27">
         <v>44.5</v>
       </c>
@@ -4478,16 +4422,16 @@
       <c r="O34" s="98"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="137"/>
+      <c r="A35" s="127"/>
       <c r="B35" s="7">
         <v>3</v>
       </c>
-      <c r="C35" s="138"/>
-      <c r="D35" s="138"/>
+      <c r="C35" s="128"/>
+      <c r="D35" s="128"/>
       <c r="E35" s="22">
         <v>35</v>
       </c>
-      <c r="F35" s="154"/>
+      <c r="F35" s="144"/>
       <c r="G35" s="27">
         <v>44.8</v>
       </c>
@@ -4510,16 +4454,16 @@
       <c r="O35" s="98"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="137"/>
+      <c r="A36" s="127"/>
       <c r="B36" s="7">
         <v>4</v>
       </c>
-      <c r="C36" s="138"/>
-      <c r="D36" s="138"/>
+      <c r="C36" s="128"/>
+      <c r="D36" s="128"/>
       <c r="E36" s="22">
         <v>36</v>
       </c>
-      <c r="F36" s="154"/>
+      <c r="F36" s="144"/>
       <c r="G36" s="27">
         <v>44.5</v>
       </c>
@@ -4542,16 +4486,16 @@
       <c r="O36" s="98"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="137"/>
+      <c r="A37" s="127"/>
       <c r="B37" s="7">
         <v>5</v>
       </c>
-      <c r="C37" s="138"/>
-      <c r="D37" s="138"/>
+      <c r="C37" s="128"/>
+      <c r="D37" s="128"/>
       <c r="E37" s="22">
         <v>37</v>
       </c>
-      <c r="F37" s="155"/>
+      <c r="F37" s="145"/>
       <c r="G37" s="27">
         <v>45.1</v>
       </c>
@@ -4574,23 +4518,23 @@
       <c r="O37" s="98"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="137">
+      <c r="A38" s="127">
         <v>8</v>
       </c>
       <c r="B38" s="7">
         <v>1</v>
       </c>
-      <c r="C38" s="138">
+      <c r="C38" s="128">
         <v>50</v>
       </c>
-      <c r="D38" s="138">
+      <c r="D38" s="128">
         <f t="shared" ref="D38" si="7">C38+273.15</f>
         <v>323.14999999999998</v>
       </c>
       <c r="E38" s="22">
         <v>38</v>
       </c>
-      <c r="F38" s="153">
+      <c r="F38" s="143">
         <v>200</v>
       </c>
       <c r="G38" s="27">
@@ -4615,16 +4559,16 @@
       <c r="O38" s="98"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="137"/>
+      <c r="A39" s="127"/>
       <c r="B39" s="7">
         <v>2</v>
       </c>
-      <c r="C39" s="138"/>
-      <c r="D39" s="138"/>
+      <c r="C39" s="128"/>
+      <c r="D39" s="128"/>
       <c r="E39" s="22">
         <v>39</v>
       </c>
-      <c r="F39" s="154"/>
+      <c r="F39" s="144"/>
       <c r="G39" s="27">
         <v>49.8</v>
       </c>
@@ -4647,16 +4591,16 @@
       <c r="O39" s="98"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="137"/>
+      <c r="A40" s="127"/>
       <c r="B40" s="7">
         <v>3</v>
       </c>
-      <c r="C40" s="138"/>
-      <c r="D40" s="138"/>
+      <c r="C40" s="128"/>
+      <c r="D40" s="128"/>
       <c r="E40" s="22">
         <v>40</v>
       </c>
-      <c r="F40" s="154"/>
+      <c r="F40" s="144"/>
       <c r="G40" s="27">
         <v>49</v>
       </c>
@@ -4679,16 +4623,16 @@
       <c r="O40" s="98"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="149"/>
+      <c r="A41" s="139"/>
       <c r="B41" s="34">
         <v>4</v>
       </c>
-      <c r="C41" s="144"/>
-      <c r="D41" s="144"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="134"/>
       <c r="E41" s="35">
         <v>41</v>
       </c>
-      <c r="F41" s="154"/>
+      <c r="F41" s="144"/>
       <c r="G41" s="36">
         <v>49.2</v>
       </c>
@@ -4711,16 +4655,16 @@
       <c r="O41" s="100"/>
     </row>
     <row r="42" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="150"/>
+      <c r="A42" s="140"/>
       <c r="B42" s="8">
         <v>5</v>
       </c>
-      <c r="C42" s="145"/>
-      <c r="D42" s="145"/>
+      <c r="C42" s="135"/>
+      <c r="D42" s="135"/>
       <c r="E42" s="23">
         <v>42</v>
       </c>
-      <c r="F42" s="156"/>
+      <c r="F42" s="146"/>
       <c r="G42" s="29">
         <v>49.7</v>
       </c>
@@ -4791,10 +4735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDC91D6-17D9-9B43-8128-D1F89723CF23}">
-  <dimension ref="A1:T42"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="R53" sqref="R53"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4802,51 +4746,47 @@
     <col min="1" max="1" width="6.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="30" style="114" customWidth="1"/>
-    <col min="15" max="15" width="25.5" style="102" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="1"/>
-    <col min="17" max="17" width="28" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="1" customWidth="1"/>
-    <col min="20" max="21" width="10.83203125" style="1"/>
-    <col min="22" max="22" width="13.5" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="18.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30" style="111" customWidth="1"/>
+    <col min="13" max="13" width="25.5" style="102" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="28" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="13.5" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="146" t="s">
+    <row r="1" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="166"/>
-      <c r="M1" s="166"/>
-      <c r="N1" s="166"/>
-      <c r="O1" s="148"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="G1" s="155"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="155"/>
+      <c r="K1" s="155"/>
+      <c r="L1" s="155"/>
+      <c r="M1" s="138"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
       <c r="Q1" s="105"/>
       <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
     </row>
-    <row r="2" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -4856,1674 +4796,1476 @@
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="110" t="s">
+      <c r="D2" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="109" t="s">
+      <c r="F2" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="115" t="s">
+      <c r="G2" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="110" t="s">
+      <c r="I2" s="110" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="121" t="s">
+      <c r="J2" s="118" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="96" t="s">
+      <c r="K2" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="121" t="s">
+      <c r="L2" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="121" t="s">
+      <c r="M2" s="118" t="s">
         <v>55</v>
       </c>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
       <c r="Q2" s="104"/>
       <c r="R2" s="104"/>
-      <c r="S2" s="104"/>
-      <c r="T2" s="104"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="164">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="154">
         <v>1</v>
       </c>
-      <c r="B3" s="122">
+      <c r="B3" s="119">
         <v>1</v>
       </c>
-      <c r="C3" s="165">
+      <c r="C3" s="129">
         <v>15</v>
       </c>
-      <c r="D3" s="165">
-        <f>C3+273.15</f>
-        <v>288.14999999999998</v>
-      </c>
-      <c r="E3" s="123">
-        <v>4</v>
-      </c>
-      <c r="F3" s="26">
+      <c r="D3" s="26">
         <v>14.75</v>
       </c>
-      <c r="G3" s="126">
-        <f>F3+274.15</f>
+      <c r="E3" s="122">
+        <f>D3+274.15</f>
         <v>288.89999999999998</v>
       </c>
-      <c r="H3" s="127">
+      <c r="F3" s="123">
         <v>25</v>
       </c>
-      <c r="I3" s="128">
+      <c r="G3" s="124">
         <v>0.3</v>
       </c>
-      <c r="J3" s="124">
+      <c r="H3" s="120">
         <v>26.6</v>
       </c>
-      <c r="K3" s="125">
+      <c r="I3" s="121">
         <v>41.6</v>
       </c>
-      <c r="L3" s="129">
+      <c r="J3" s="125">
         <v>5.94E-3</v>
       </c>
-      <c r="M3" s="158">
-        <f>AVERAGE(L3:L7)</f>
+      <c r="K3" s="148">
+        <f>AVERAGE(J3:J7)</f>
         <v>1.0232E-2</v>
       </c>
-      <c r="N3" s="161">
-        <f>O3/SQRT(5)</f>
+      <c r="L3" s="151">
+        <f>M3/SQRT(5)</f>
         <v>1.9391271232180748E-3</v>
       </c>
-      <c r="O3" s="161">
-        <f>_xlfn.STDEV.S(L3:L7)</f>
+      <c r="M3" s="151">
+        <f>_xlfn.STDEV.S(J3:J7)</f>
         <v>4.336020064529226E-3</v>
       </c>
-      <c r="S3" s="167"/>
+      <c r="Q3" s="156"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="137"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="127"/>
       <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="138"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="111">
-        <v>5</v>
-      </c>
-      <c r="F4" s="26">
+      <c r="C4" s="128"/>
+      <c r="D4" s="26">
         <v>15.7</v>
       </c>
-      <c r="G4" s="26">
-        <f t="shared" ref="G4:G42" si="0">F4+274.15</f>
+      <c r="E4" s="26">
+        <f t="shared" ref="E4:E42" si="0">D4+274.15</f>
         <v>289.84999999999997</v>
       </c>
-      <c r="H4" s="106">
+      <c r="F4" s="106">
         <v>25</v>
       </c>
-      <c r="I4" s="116">
+      <c r="G4" s="113">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J4" s="27">
+      <c r="H4" s="27">
         <v>40.4</v>
       </c>
-      <c r="K4" s="17">
+      <c r="I4" s="17">
         <v>55.4</v>
       </c>
-      <c r="L4" s="119">
+      <c r="J4" s="116">
         <v>8.1700000000000002E-3</v>
       </c>
-      <c r="M4" s="159"/>
-      <c r="N4" s="162"/>
-      <c r="O4" s="162"/>
-      <c r="S4" s="167"/>
+      <c r="K4" s="149"/>
+      <c r="L4" s="152"/>
+      <c r="M4" s="152"/>
+      <c r="Q4" s="156"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="137"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="127"/>
       <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="138"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="111">
-        <v>6</v>
-      </c>
-      <c r="F5" s="26">
+      <c r="C5" s="128"/>
+      <c r="D5" s="26">
         <v>14.35</v>
       </c>
-      <c r="G5" s="26">
+      <c r="E5" s="26">
         <f t="shared" si="0"/>
         <v>288.5</v>
       </c>
-      <c r="H5" s="106">
+      <c r="F5" s="106">
         <v>25</v>
       </c>
-      <c r="I5" s="116">
+      <c r="G5" s="113">
         <v>0.32</v>
       </c>
-      <c r="J5" s="27">
+      <c r="H5" s="27">
         <v>30</v>
       </c>
-      <c r="K5" s="17">
+      <c r="I5" s="17">
         <v>45</v>
       </c>
-      <c r="L5" s="119">
+      <c r="J5" s="116">
         <v>1.2370000000000001E-2</v>
       </c>
-      <c r="M5" s="159"/>
-      <c r="N5" s="162"/>
-      <c r="O5" s="162"/>
+      <c r="K5" s="149"/>
+      <c r="L5" s="152"/>
+      <c r="M5" s="152"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="137"/>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="127"/>
       <c r="B6" s="7">
         <v>4</v>
       </c>
-      <c r="C6" s="138"/>
-      <c r="D6" s="138"/>
-      <c r="E6" s="111">
-        <v>7</v>
-      </c>
-      <c r="F6" s="26">
+      <c r="C6" s="128"/>
+      <c r="D6" s="26">
         <v>15.100000000000001</v>
       </c>
-      <c r="G6" s="26">
+      <c r="E6" s="26">
         <f t="shared" si="0"/>
         <v>289.25</v>
       </c>
-      <c r="H6" s="106">
+      <c r="F6" s="106">
         <v>25</v>
       </c>
-      <c r="I6" s="116">
+      <c r="G6" s="113">
         <v>0.32</v>
       </c>
-      <c r="J6" s="27">
+      <c r="H6" s="27">
         <v>30</v>
       </c>
-      <c r="K6" s="17">
+      <c r="I6" s="17">
         <v>45</v>
       </c>
-      <c r="L6" s="119">
+      <c r="J6" s="116">
         <v>1.6760000000000001E-2</v>
       </c>
-      <c r="M6" s="159"/>
-      <c r="N6" s="162"/>
-      <c r="O6" s="162"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="152"/>
+      <c r="M6" s="152"/>
     </row>
-    <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="150"/>
-      <c r="B7" s="130">
+    <row r="7" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="140"/>
+      <c r="B7" s="126">
         <v>5</v>
       </c>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="131">
-        <v>8</v>
-      </c>
-      <c r="F7" s="93">
+      <c r="C7" s="128"/>
+      <c r="D7" s="26">
         <v>14.86</v>
       </c>
-      <c r="G7" s="133">
+      <c r="E7" s="103">
         <f t="shared" si="0"/>
         <v>289.01</v>
       </c>
-      <c r="H7" s="134">
+      <c r="F7" s="172">
         <v>25</v>
       </c>
-      <c r="I7" s="135">
+      <c r="G7" s="115">
         <v>0.31</v>
       </c>
-      <c r="J7" s="132">
+      <c r="H7" s="29">
         <v>20.2</v>
       </c>
-      <c r="K7" s="68">
+      <c r="I7" s="18">
         <v>35.200000000000003</v>
       </c>
-      <c r="L7" s="136">
+      <c r="J7" s="117">
         <v>7.92E-3</v>
       </c>
-      <c r="M7" s="160"/>
-      <c r="N7" s="163"/>
-      <c r="O7" s="163"/>
+      <c r="K7" s="150"/>
+      <c r="L7" s="153"/>
+      <c r="M7" s="153"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="164">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="154">
         <v>2</v>
       </c>
-      <c r="B8" s="122">
+      <c r="B8" s="119">
         <v>1</v>
       </c>
-      <c r="C8" s="165">
+      <c r="C8" s="128">
         <v>20</v>
       </c>
-      <c r="D8" s="165">
-        <f t="shared" ref="D8" si="1">C8+273.15</f>
-        <v>293.14999999999998</v>
-      </c>
-      <c r="E8" s="123">
-        <v>48</v>
-      </c>
-      <c r="F8" s="26">
+      <c r="D8" s="26">
         <v>19</v>
       </c>
-      <c r="G8" s="126">
+      <c r="E8" s="122">
         <f t="shared" si="0"/>
         <v>293.14999999999998</v>
       </c>
-      <c r="H8" s="127">
+      <c r="F8" s="123">
         <v>25</v>
       </c>
-      <c r="I8" s="128">
+      <c r="G8" s="124">
         <v>0.3</v>
       </c>
-      <c r="J8" s="124">
+      <c r="H8" s="120">
         <v>31.8</v>
       </c>
-      <c r="K8" s="125">
+      <c r="I8" s="121">
         <v>46.8</v>
       </c>
-      <c r="L8" s="129">
+      <c r="J8" s="125">
         <v>1.397E-2</v>
       </c>
-      <c r="M8" s="158">
-        <f t="shared" ref="M8" si="2">AVERAGE(L8:L12)</f>
+      <c r="K8" s="148">
+        <f t="shared" ref="K8" si="1">AVERAGE(J8:J12)</f>
         <v>1.4062E-2</v>
       </c>
-      <c r="N8" s="161">
-        <f t="shared" ref="N8" si="3">O8/SQRT(5)</f>
+      <c r="L8" s="151">
+        <f t="shared" ref="L8" si="2">M8/SQRT(5)</f>
         <v>2.2252806564566183E-3</v>
       </c>
-      <c r="O8" s="161">
-        <f t="shared" ref="O8" si="4">_xlfn.STDEV.S(L8:L12)</f>
+      <c r="M8" s="151">
+        <f t="shared" ref="M8" si="3">_xlfn.STDEV.S(J8:J12)</f>
         <v>4.9758788168523553E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="137"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="127"/>
       <c r="B9" s="7">
         <v>2</v>
       </c>
-      <c r="C9" s="138"/>
-      <c r="D9" s="138"/>
-      <c r="E9" s="111">
-        <v>9</v>
-      </c>
-      <c r="F9" s="26">
+      <c r="C9" s="128"/>
+      <c r="D9" s="26">
         <v>20.95</v>
       </c>
-      <c r="G9" s="26">
+      <c r="E9" s="26">
         <f t="shared" si="0"/>
         <v>295.09999999999997</v>
       </c>
-      <c r="H9" s="107">
+      <c r="F9" s="107">
         <v>25</v>
       </c>
-      <c r="I9" s="116">
+      <c r="G9" s="113">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J9" s="27">
+      <c r="H9" s="27">
         <v>17.2</v>
       </c>
-      <c r="K9" s="17">
+      <c r="I9" s="17">
         <v>32.200000000000003</v>
       </c>
-      <c r="L9" s="119">
+      <c r="J9" s="116">
         <v>8.6400000000000001E-3</v>
       </c>
-      <c r="M9" s="159"/>
-      <c r="N9" s="162"/>
-      <c r="O9" s="162"/>
+      <c r="K9" s="149"/>
+      <c r="L9" s="152"/>
+      <c r="M9" s="152"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="137"/>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="127"/>
       <c r="B10" s="7">
         <v>3</v>
       </c>
-      <c r="C10" s="138"/>
-      <c r="D10" s="138"/>
-      <c r="E10" s="111">
-        <v>10</v>
-      </c>
-      <c r="F10" s="26">
+      <c r="C10" s="128"/>
+      <c r="D10" s="26">
         <v>21.15</v>
       </c>
-      <c r="G10" s="26">
+      <c r="E10" s="26">
         <f t="shared" si="0"/>
         <v>295.29999999999995</v>
       </c>
-      <c r="H10" s="107">
+      <c r="F10" s="107">
         <v>25</v>
       </c>
-      <c r="I10" s="116">
+      <c r="G10" s="113">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J10" s="27">
+      <c r="H10" s="27">
         <v>25.8</v>
       </c>
-      <c r="K10" s="17">
+      <c r="I10" s="17">
         <v>40.799999999999997</v>
       </c>
-      <c r="L10" s="119">
+      <c r="J10" s="116">
         <v>1.5100000000000001E-2</v>
       </c>
-      <c r="M10" s="159"/>
-      <c r="N10" s="162"/>
-      <c r="O10" s="162"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="152"/>
+      <c r="M10" s="152"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="137"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="127"/>
       <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="138"/>
-      <c r="D11" s="138"/>
-      <c r="E11" s="111">
-        <v>11</v>
-      </c>
-      <c r="F11" s="26">
+      <c r="C11" s="128"/>
+      <c r="D11" s="26">
         <v>19.549999999999997</v>
       </c>
-      <c r="G11" s="26">
+      <c r="E11" s="26">
         <f t="shared" si="0"/>
         <v>293.7</v>
       </c>
-      <c r="H11" s="107">
+      <c r="F11" s="107">
         <v>25</v>
       </c>
-      <c r="I11" s="116">
+      <c r="G11" s="113">
         <v>0.31</v>
       </c>
-      <c r="J11" s="27">
+      <c r="H11" s="27">
         <v>30</v>
       </c>
-      <c r="K11" s="17">
+      <c r="I11" s="17">
         <v>45</v>
       </c>
-      <c r="L11" s="119">
+      <c r="J11" s="116">
         <v>2.171E-2</v>
       </c>
-      <c r="M11" s="159"/>
-      <c r="N11" s="162"/>
-      <c r="O11" s="162"/>
+      <c r="K11" s="149"/>
+      <c r="L11" s="152"/>
+      <c r="M11" s="152"/>
     </row>
-    <row r="12" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="150"/>
+    <row r="12" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="140"/>
       <c r="B12" s="8">
         <v>5</v>
       </c>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="113">
-        <v>12</v>
-      </c>
-      <c r="F12" s="26">
+      <c r="C12" s="128"/>
+      <c r="D12" s="26">
         <v>19.55</v>
       </c>
-      <c r="G12" s="103">
+      <c r="E12" s="103">
         <f t="shared" si="0"/>
         <v>293.7</v>
       </c>
-      <c r="H12" s="108">
+      <c r="F12" s="108">
         <v>25</v>
       </c>
-      <c r="I12" s="118">
+      <c r="G12" s="115">
         <v>0.31</v>
       </c>
-      <c r="J12" s="29">
+      <c r="H12" s="29">
         <v>24</v>
       </c>
-      <c r="K12" s="18">
+      <c r="I12" s="18">
         <v>39</v>
       </c>
-      <c r="L12" s="120">
+      <c r="J12" s="117">
         <v>1.089E-2</v>
       </c>
-      <c r="M12" s="160"/>
-      <c r="N12" s="163"/>
-      <c r="O12" s="163"/>
+      <c r="K12" s="150"/>
+      <c r="L12" s="153"/>
+      <c r="M12" s="153"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="164">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="154">
         <v>3</v>
       </c>
-      <c r="B13" s="122">
+      <c r="B13" s="119">
         <v>1</v>
       </c>
-      <c r="C13" s="165">
+      <c r="C13" s="128">
         <v>25</v>
       </c>
-      <c r="D13" s="165">
-        <f t="shared" ref="D13" si="5">C13+273.15</f>
-        <v>298.14999999999998</v>
-      </c>
-      <c r="E13" s="123">
-        <v>13</v>
-      </c>
-      <c r="F13" s="26">
+      <c r="D13" s="26">
         <v>25.5</v>
       </c>
-      <c r="G13" s="126">
+      <c r="E13" s="122">
         <f t="shared" si="0"/>
         <v>299.64999999999998</v>
       </c>
-      <c r="H13" s="127">
+      <c r="F13" s="123">
         <v>25</v>
       </c>
-      <c r="I13" s="128">
+      <c r="G13" s="124">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J13" s="124">
+      <c r="H13" s="120">
         <v>19</v>
       </c>
-      <c r="K13" s="125">
+      <c r="I13" s="121">
         <v>34</v>
       </c>
-      <c r="L13" s="129">
+      <c r="J13" s="125">
         <v>1.8669999999999999E-2</v>
       </c>
-      <c r="M13" s="158">
-        <f t="shared" ref="M13" si="6">AVERAGE(L13:L17)</f>
+      <c r="K13" s="148">
+        <f t="shared" ref="K13" si="4">AVERAGE(J13:J17)</f>
         <v>1.7819999999999996E-2</v>
       </c>
-      <c r="N13" s="161">
-        <f t="shared" ref="N13" si="7">O13/SQRT(5)</f>
+      <c r="L13" s="151">
+        <f t="shared" ref="L13" si="5">M13/SQRT(5)</f>
         <v>3.1548993644805894E-3</v>
       </c>
-      <c r="O13" s="161">
-        <f t="shared" ref="O13" si="8">_xlfn.STDEV.S(L13:L17)</f>
+      <c r="M13" s="151">
+        <f t="shared" ref="M13" si="6">_xlfn.STDEV.S(J13:J17)</f>
         <v>7.0545694411494834E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="137"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="127"/>
       <c r="B14" s="7">
         <v>2</v>
       </c>
-      <c r="C14" s="138"/>
-      <c r="D14" s="138"/>
-      <c r="E14" s="111">
-        <v>14</v>
-      </c>
-      <c r="F14" s="26">
+      <c r="C14" s="128"/>
+      <c r="D14" s="26">
         <v>25.55</v>
       </c>
-      <c r="G14" s="26">
+      <c r="E14" s="26">
         <f t="shared" si="0"/>
         <v>299.7</v>
       </c>
-      <c r="H14" s="107">
+      <c r="F14" s="107">
         <v>25</v>
       </c>
-      <c r="I14" s="116">
+      <c r="G14" s="113">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J14" s="27">
+      <c r="H14" s="27">
         <v>20</v>
       </c>
-      <c r="K14" s="17">
+      <c r="I14" s="17">
         <v>35</v>
       </c>
-      <c r="L14" s="119">
+      <c r="J14" s="116">
         <v>2.8639999999999999E-2</v>
       </c>
-      <c r="M14" s="159"/>
-      <c r="N14" s="162"/>
-      <c r="O14" s="162"/>
+      <c r="K14" s="149"/>
+      <c r="L14" s="152"/>
+      <c r="M14" s="152"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="137"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="127"/>
       <c r="B15" s="7">
         <v>3</v>
       </c>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="111">
-        <v>15</v>
-      </c>
-      <c r="F15" s="26">
+      <c r="C15" s="128"/>
+      <c r="D15" s="26">
         <v>26.2</v>
       </c>
-      <c r="G15" s="26">
+      <c r="E15" s="26">
         <f t="shared" si="0"/>
         <v>300.34999999999997</v>
       </c>
-      <c r="H15" s="107">
+      <c r="F15" s="107">
         <v>25</v>
       </c>
-      <c r="I15" s="116">
+      <c r="G15" s="113">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J15" s="27">
+      <c r="H15" s="27">
         <v>27.2</v>
       </c>
-      <c r="K15" s="17">
+      <c r="I15" s="17">
         <v>42.2</v>
       </c>
-      <c r="L15" s="119">
+      <c r="J15" s="116">
         <v>1.6310000000000002E-2</v>
       </c>
-      <c r="M15" s="159"/>
-      <c r="N15" s="162"/>
-      <c r="O15" s="162"/>
+      <c r="K15" s="149"/>
+      <c r="L15" s="152"/>
+      <c r="M15" s="152"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="137"/>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="127"/>
       <c r="B16" s="7">
         <v>4</v>
       </c>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="111">
-        <v>16</v>
-      </c>
-      <c r="F16" s="26">
+      <c r="C16" s="128"/>
+      <c r="D16" s="26">
         <v>24.65</v>
       </c>
-      <c r="G16" s="26">
+      <c r="E16" s="26">
         <f t="shared" si="0"/>
         <v>298.79999999999995</v>
       </c>
-      <c r="H16" s="107">
+      <c r="F16" s="107">
         <v>25</v>
       </c>
-      <c r="I16" s="116">
+      <c r="G16" s="113">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J16" s="27">
+      <c r="H16" s="27">
         <v>24</v>
       </c>
-      <c r="K16" s="17">
+      <c r="I16" s="17">
         <v>39</v>
       </c>
-      <c r="L16" s="119">
+      <c r="J16" s="116">
         <v>1.644E-2</v>
       </c>
-      <c r="M16" s="159"/>
-      <c r="N16" s="162"/>
-      <c r="O16" s="162"/>
+      <c r="K16" s="149"/>
+      <c r="L16" s="152"/>
+      <c r="M16" s="152"/>
     </row>
-    <row r="17" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="150"/>
+    <row r="17" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="140"/>
       <c r="B17" s="8">
         <v>5</v>
       </c>
-      <c r="C17" s="145"/>
-      <c r="D17" s="145"/>
-      <c r="E17" s="113">
-        <v>17</v>
-      </c>
-      <c r="F17" s="26">
+      <c r="C17" s="128"/>
+      <c r="D17" s="26">
         <v>25.65</v>
       </c>
-      <c r="G17" s="103">
+      <c r="E17" s="103">
         <f t="shared" si="0"/>
         <v>299.79999999999995</v>
       </c>
-      <c r="H17" s="108">
+      <c r="F17" s="108">
         <v>25</v>
       </c>
-      <c r="I17" s="118">
+      <c r="G17" s="115">
         <v>0.3</v>
       </c>
-      <c r="J17" s="29">
+      <c r="H17" s="29">
         <v>20</v>
       </c>
-      <c r="K17" s="18">
+      <c r="I17" s="18">
         <v>35</v>
       </c>
-      <c r="L17" s="120">
+      <c r="J17" s="117">
         <v>9.0399999999999994E-3</v>
       </c>
-      <c r="M17" s="160"/>
-      <c r="N17" s="163"/>
-      <c r="O17" s="163"/>
+      <c r="K17" s="150"/>
+      <c r="L17" s="153"/>
+      <c r="M17" s="153"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="164">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="154">
         <v>4</v>
       </c>
-      <c r="B18" s="122">
+      <c r="B18" s="119">
         <v>1</v>
       </c>
-      <c r="C18" s="165">
+      <c r="C18" s="128">
         <v>30</v>
       </c>
-      <c r="D18" s="165">
-        <f t="shared" ref="D18" si="9">C18+273.15</f>
-        <v>303.14999999999998</v>
-      </c>
-      <c r="E18" s="123">
-        <v>18</v>
-      </c>
-      <c r="F18" s="26">
+      <c r="D18" s="26">
         <v>30.1</v>
       </c>
-      <c r="G18" s="126">
+      <c r="E18" s="122">
         <f t="shared" si="0"/>
         <v>304.25</v>
       </c>
-      <c r="H18" s="127">
+      <c r="F18" s="123">
         <v>25</v>
       </c>
-      <c r="I18" s="128">
+      <c r="G18" s="124">
         <v>0.33</v>
       </c>
-      <c r="J18" s="124">
+      <c r="H18" s="120">
         <v>5.6</v>
       </c>
-      <c r="K18" s="125">
+      <c r="I18" s="121">
         <v>20.6</v>
       </c>
-      <c r="L18" s="129">
+      <c r="J18" s="125">
         <v>3.8109999999999998E-2</v>
       </c>
-      <c r="M18" s="158">
-        <f t="shared" ref="M18" si="10">AVERAGE(L18:L22)</f>
+      <c r="K18" s="148">
+        <f t="shared" ref="K18" si="7">AVERAGE(J18:J22)</f>
         <v>3.8837999999999998E-2</v>
       </c>
-      <c r="N18" s="161">
-        <f t="shared" ref="N18" si="11">O18/SQRT(5)</f>
+      <c r="L18" s="151">
+        <f t="shared" ref="L18" si="8">M18/SQRT(5)</f>
         <v>8.6950131684776603E-3</v>
       </c>
-      <c r="O18" s="161">
-        <f t="shared" ref="O18" si="12">_xlfn.STDEV.S(L18:L22)</f>
+      <c r="M18" s="151">
+        <f t="shared" ref="M18" si="9">_xlfn.STDEV.S(J18:J22)</f>
         <v>1.9442640509971881E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="137"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="127"/>
       <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="111">
-        <v>19</v>
-      </c>
-      <c r="F19" s="26">
+      <c r="C19" s="128"/>
+      <c r="D19" s="26">
         <v>28.8</v>
       </c>
-      <c r="G19" s="26">
+      <c r="E19" s="26">
         <f t="shared" si="0"/>
         <v>302.95</v>
       </c>
-      <c r="H19" s="107">
+      <c r="F19" s="107">
         <v>25</v>
       </c>
-      <c r="I19" s="116">
+      <c r="G19" s="113">
         <v>0.3</v>
       </c>
-      <c r="J19" s="27">
+      <c r="H19" s="27">
         <v>10.199999999999999</v>
       </c>
-      <c r="K19" s="17">
+      <c r="I19" s="17">
         <v>25.2</v>
       </c>
-      <c r="L19" s="119">
+      <c r="J19" s="116">
         <v>2.3269999999999999E-2</v>
       </c>
-      <c r="M19" s="159"/>
-      <c r="N19" s="162"/>
-      <c r="O19" s="162"/>
+      <c r="K19" s="149"/>
+      <c r="L19" s="152"/>
+      <c r="M19" s="152"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="137"/>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="127"/>
       <c r="B20" s="7">
         <v>3</v>
       </c>
-      <c r="C20" s="138"/>
-      <c r="D20" s="138"/>
-      <c r="E20" s="111">
-        <v>20</v>
-      </c>
-      <c r="F20" s="26">
+      <c r="C20" s="128"/>
+      <c r="D20" s="26">
         <v>31.2</v>
       </c>
-      <c r="G20" s="26">
+      <c r="E20" s="26">
         <f t="shared" si="0"/>
         <v>305.34999999999997</v>
       </c>
-      <c r="H20" s="107">
+      <c r="F20" s="107">
         <v>25</v>
       </c>
-      <c r="I20" s="116">
+      <c r="G20" s="113">
         <v>0.3</v>
       </c>
-      <c r="J20" s="27">
+      <c r="H20" s="27">
         <v>11</v>
       </c>
-      <c r="K20" s="17">
+      <c r="I20" s="17">
         <v>26</v>
       </c>
-      <c r="L20" s="119">
+      <c r="J20" s="116">
         <v>6.7760000000000001E-2</v>
       </c>
-      <c r="M20" s="159"/>
-      <c r="N20" s="162"/>
-      <c r="O20" s="162"/>
+      <c r="K20" s="149"/>
+      <c r="L20" s="152"/>
+      <c r="M20" s="152"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="137"/>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="127"/>
       <c r="B21" s="7">
         <v>4</v>
       </c>
-      <c r="C21" s="138"/>
-      <c r="D21" s="138"/>
-      <c r="E21" s="111">
-        <v>21</v>
-      </c>
-      <c r="F21" s="26">
+      <c r="C21" s="128"/>
+      <c r="D21" s="26">
         <v>30.2</v>
       </c>
-      <c r="G21" s="26">
+      <c r="E21" s="26">
         <f t="shared" si="0"/>
         <v>304.34999999999997</v>
       </c>
-      <c r="H21" s="107">
+      <c r="F21" s="107">
         <v>25</v>
       </c>
-      <c r="I21" s="116">
+      <c r="G21" s="113">
         <v>0.3</v>
       </c>
-      <c r="J21" s="27">
+      <c r="H21" s="27">
         <v>17.2</v>
       </c>
-      <c r="K21" s="17">
+      <c r="I21" s="17">
         <v>32.200000000000003</v>
       </c>
-      <c r="L21" s="119">
+      <c r="J21" s="116">
         <v>4.5809999999999997E-2</v>
       </c>
-      <c r="M21" s="159"/>
-      <c r="N21" s="162"/>
-      <c r="O21" s="162"/>
+      <c r="K21" s="149"/>
+      <c r="L21" s="152"/>
+      <c r="M21" s="152"/>
     </row>
-    <row r="22" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
+    <row r="22" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="140"/>
       <c r="B22" s="8">
         <v>5</v>
       </c>
-      <c r="C22" s="145"/>
-      <c r="D22" s="145"/>
-      <c r="E22" s="113">
-        <v>22</v>
-      </c>
-      <c r="F22" s="26">
+      <c r="C22" s="128"/>
+      <c r="D22" s="26">
         <v>30.9</v>
       </c>
-      <c r="G22" s="103">
+      <c r="E22" s="103">
         <f t="shared" si="0"/>
         <v>305.04999999999995</v>
       </c>
-      <c r="H22" s="108">
+      <c r="F22" s="108">
         <v>25</v>
       </c>
-      <c r="I22" s="118">
+      <c r="G22" s="115">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J22" s="29">
+      <c r="H22" s="29">
         <v>11.4</v>
       </c>
-      <c r="K22" s="18">
+      <c r="I22" s="18">
         <v>26.4</v>
       </c>
-      <c r="L22" s="120">
+      <c r="J22" s="117">
         <v>1.924E-2</v>
       </c>
-      <c r="M22" s="160"/>
-      <c r="N22" s="163"/>
-      <c r="O22" s="163"/>
+      <c r="K22" s="150"/>
+      <c r="L22" s="153"/>
+      <c r="M22" s="153"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="164">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="154">
         <v>5</v>
       </c>
-      <c r="B23" s="122">
+      <c r="B23" s="119">
         <v>1</v>
       </c>
-      <c r="C23" s="165">
+      <c r="C23" s="128">
         <v>35</v>
       </c>
-      <c r="D23" s="165">
-        <f t="shared" ref="D23" si="13">C23+273.15</f>
-        <v>308.14999999999998</v>
-      </c>
-      <c r="E23" s="123">
-        <v>23</v>
-      </c>
-      <c r="F23" s="26">
+      <c r="D23" s="26">
         <v>35.5</v>
       </c>
-      <c r="G23" s="126">
+      <c r="E23" s="122">
         <f t="shared" si="0"/>
         <v>309.64999999999998</v>
       </c>
-      <c r="H23" s="127">
+      <c r="F23" s="123">
         <v>25</v>
       </c>
-      <c r="I23" s="128">
+      <c r="G23" s="124">
         <v>0.31</v>
       </c>
-      <c r="J23" s="124">
+      <c r="H23" s="120">
         <v>8</v>
       </c>
-      <c r="K23" s="125">
+      <c r="I23" s="121">
         <v>23</v>
       </c>
-      <c r="L23" s="129">
+      <c r="J23" s="125">
         <v>6.9919999999999996E-2</v>
       </c>
-      <c r="M23" s="158">
-        <f t="shared" ref="M23" si="14">AVERAGE(L23:L27)</f>
+      <c r="K23" s="148">
+        <f t="shared" ref="K23" si="10">AVERAGE(J23:J27)</f>
         <v>5.4418000000000001E-2</v>
       </c>
-      <c r="N23" s="161">
-        <f t="shared" ref="N23" si="15">O23/SQRT(5)</f>
+      <c r="L23" s="151">
+        <f t="shared" ref="L23" si="11">M23/SQRT(5)</f>
         <v>6.0011560552946722E-3</v>
       </c>
-      <c r="O23" s="161">
-        <f t="shared" ref="O23" si="16">_xlfn.STDEV.S(L23:L27)</f>
+      <c r="M23" s="151">
+        <f t="shared" ref="M23" si="12">_xlfn.STDEV.S(J23:J27)</f>
         <v>1.3418992883223374E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="137"/>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="127"/>
       <c r="B24" s="7">
         <v>2</v>
       </c>
-      <c r="C24" s="138"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="111">
-        <v>24</v>
-      </c>
-      <c r="F24" s="26">
+      <c r="C24" s="128"/>
+      <c r="D24" s="26">
         <v>35.549999999999997</v>
       </c>
-      <c r="G24" s="26">
+      <c r="E24" s="26">
         <f t="shared" si="0"/>
         <v>309.7</v>
       </c>
-      <c r="H24" s="107">
+      <c r="F24" s="107">
         <v>25</v>
       </c>
-      <c r="I24" s="116">
+      <c r="G24" s="113">
         <v>0.31</v>
       </c>
-      <c r="J24" s="27">
+      <c r="H24" s="27">
         <v>16.8</v>
       </c>
-      <c r="K24" s="17">
+      <c r="I24" s="17">
         <v>31.8</v>
       </c>
-      <c r="L24" s="119">
+      <c r="J24" s="116">
         <v>5.917E-2</v>
       </c>
-      <c r="M24" s="159"/>
-      <c r="N24" s="162"/>
-      <c r="O24" s="162"/>
+      <c r="K24" s="149"/>
+      <c r="L24" s="152"/>
+      <c r="M24" s="152"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="137"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="127"/>
       <c r="B25" s="7">
         <v>3</v>
       </c>
-      <c r="C25" s="138"/>
-      <c r="D25" s="138"/>
-      <c r="E25" s="111">
-        <v>25</v>
-      </c>
-      <c r="F25" s="26">
+      <c r="C25" s="128"/>
+      <c r="D25" s="26">
         <v>34.200000000000003</v>
       </c>
-      <c r="G25" s="26">
+      <c r="E25" s="26">
         <f t="shared" si="0"/>
         <v>308.34999999999997</v>
       </c>
-      <c r="H25" s="107">
+      <c r="F25" s="107">
         <v>25</v>
       </c>
-      <c r="I25" s="116">
+      <c r="G25" s="113">
         <v>0.32</v>
       </c>
-      <c r="J25" s="27">
+      <c r="H25" s="27">
         <v>13.2</v>
       </c>
-      <c r="K25" s="17">
+      <c r="I25" s="17">
         <v>28.2</v>
       </c>
-      <c r="L25" s="119">
+      <c r="J25" s="116">
         <v>6.2269999999999999E-2</v>
       </c>
-      <c r="M25" s="159"/>
-      <c r="N25" s="162"/>
-      <c r="O25" s="162"/>
+      <c r="K25" s="149"/>
+      <c r="L25" s="152"/>
+      <c r="M25" s="152"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="137"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="127"/>
       <c r="B26" s="7">
         <v>4</v>
       </c>
-      <c r="C26" s="138"/>
-      <c r="D26" s="138"/>
-      <c r="E26" s="111">
-        <v>26</v>
-      </c>
-      <c r="F26" s="26">
+      <c r="C26" s="128"/>
+      <c r="D26" s="26">
         <v>35</v>
       </c>
-      <c r="G26" s="26">
+      <c r="E26" s="26">
         <f t="shared" si="0"/>
         <v>309.14999999999998</v>
       </c>
-      <c r="H26" s="107">
+      <c r="F26" s="107">
         <v>25</v>
       </c>
-      <c r="I26" s="116">
+      <c r="G26" s="113">
         <v>0.31</v>
       </c>
-      <c r="J26" s="27">
+      <c r="H26" s="27">
         <v>6.2</v>
       </c>
-      <c r="K26" s="17">
+      <c r="I26" s="17">
         <v>21.2</v>
       </c>
-      <c r="L26" s="119">
+      <c r="J26" s="116">
         <v>4.0980000000000003E-2</v>
       </c>
-      <c r="M26" s="159"/>
-      <c r="N26" s="162"/>
-      <c r="O26" s="162"/>
+      <c r="K26" s="149"/>
+      <c r="L26" s="152"/>
+      <c r="M26" s="152"/>
     </row>
-    <row r="27" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="150"/>
+    <row r="27" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="140"/>
       <c r="B27" s="8">
         <v>5</v>
       </c>
-      <c r="C27" s="145"/>
-      <c r="D27" s="145"/>
-      <c r="E27" s="113">
-        <v>27</v>
-      </c>
-      <c r="F27" s="26">
+      <c r="C27" s="128"/>
+      <c r="D27" s="26">
         <v>35.9</v>
       </c>
-      <c r="G27" s="103">
+      <c r="E27" s="103">
         <f t="shared" si="0"/>
         <v>310.04999999999995</v>
       </c>
-      <c r="H27" s="108">
+      <c r="F27" s="108">
         <v>25</v>
       </c>
-      <c r="I27" s="118">
+      <c r="G27" s="115">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J27" s="29">
+      <c r="H27" s="29">
         <v>21.4</v>
       </c>
-      <c r="K27" s="18">
+      <c r="I27" s="18">
         <v>36.4</v>
       </c>
-      <c r="L27" s="120">
+      <c r="J27" s="117">
         <v>3.9750000000000001E-2</v>
       </c>
-      <c r="M27" s="160"/>
-      <c r="N27" s="163"/>
-      <c r="O27" s="163"/>
+      <c r="K27" s="150"/>
+      <c r="L27" s="153"/>
+      <c r="M27" s="153"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="164">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="154">
         <v>6</v>
       </c>
-      <c r="B28" s="122">
+      <c r="B28" s="119">
         <v>1</v>
       </c>
-      <c r="C28" s="165">
+      <c r="C28" s="128">
         <v>40</v>
       </c>
-      <c r="D28" s="165">
-        <f t="shared" ref="D28" si="17">C28+273.15</f>
-        <v>313.14999999999998</v>
-      </c>
-      <c r="E28" s="123">
-        <v>43</v>
-      </c>
-      <c r="F28" s="26">
+      <c r="D28" s="26">
         <v>40.349999999999994</v>
       </c>
-      <c r="G28" s="126">
+      <c r="E28" s="122">
         <f t="shared" si="0"/>
         <v>314.5</v>
       </c>
-      <c r="H28" s="127">
+      <c r="F28" s="123">
         <v>25</v>
       </c>
-      <c r="I28" s="128">
+      <c r="G28" s="124">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J28" s="124">
+      <c r="H28" s="120">
         <v>11.6</v>
       </c>
-      <c r="K28" s="125">
+      <c r="I28" s="121">
         <v>26.6</v>
       </c>
-      <c r="L28" s="129">
+      <c r="J28" s="125">
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="M28" s="158">
-        <f t="shared" ref="M28" si="18">AVERAGE(L28:L32)</f>
+      <c r="K28" s="148">
+        <f t="shared" ref="K28" si="13">AVERAGE(J28:J32)</f>
         <v>4.2141999999999999E-2</v>
       </c>
-      <c r="N28" s="161">
-        <f t="shared" ref="N28" si="19">O28/SQRT(5)</f>
+      <c r="L28" s="151">
+        <f t="shared" ref="L28" si="14">M28/SQRT(5)</f>
         <v>8.2617494515387011E-3</v>
       </c>
-      <c r="O28" s="161">
-        <f t="shared" ref="O28" si="20">_xlfn.STDEV.S(L28:L32)</f>
+      <c r="M28" s="151">
+        <f t="shared" ref="M28" si="15">_xlfn.STDEV.S(J28:J32)</f>
         <v>1.847383338671214E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="137"/>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="127"/>
       <c r="B29" s="7">
         <v>2</v>
       </c>
-      <c r="C29" s="138"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="111">
-        <v>44</v>
-      </c>
-      <c r="F29" s="26">
+      <c r="C29" s="128"/>
+      <c r="D29" s="26">
         <v>41.2</v>
       </c>
-      <c r="G29" s="26">
+      <c r="E29" s="26">
         <f t="shared" si="0"/>
         <v>315.34999999999997</v>
       </c>
-      <c r="H29" s="107">
+      <c r="F29" s="107">
         <v>25</v>
       </c>
-      <c r="I29" s="116">
+      <c r="G29" s="113">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J29" s="27">
+      <c r="H29" s="27">
         <v>11</v>
       </c>
-      <c r="K29" s="17">
+      <c r="I29" s="17">
         <v>26</v>
       </c>
-      <c r="L29" s="119">
+      <c r="J29" s="116">
         <v>2.9139999999999999E-2</v>
       </c>
-      <c r="M29" s="159"/>
-      <c r="N29" s="162"/>
-      <c r="O29" s="162"/>
+      <c r="K29" s="149"/>
+      <c r="L29" s="152"/>
+      <c r="M29" s="152"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="137"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="127"/>
       <c r="B30" s="7">
         <v>3</v>
       </c>
-      <c r="C30" s="138"/>
-      <c r="D30" s="138"/>
-      <c r="E30" s="111">
-        <v>45</v>
-      </c>
-      <c r="F30" s="26">
+      <c r="C30" s="128"/>
+      <c r="D30" s="26">
         <v>38.9</v>
       </c>
-      <c r="G30" s="26">
+      <c r="E30" s="26">
         <f t="shared" si="0"/>
         <v>313.04999999999995</v>
       </c>
-      <c r="H30" s="107">
+      <c r="F30" s="107">
         <v>25</v>
       </c>
-      <c r="I30" s="116">
+      <c r="G30" s="113">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J30" s="27">
+      <c r="H30" s="27">
         <v>9.6</v>
       </c>
-      <c r="K30" s="17">
+      <c r="I30" s="17">
         <v>24.6</v>
       </c>
-      <c r="L30" s="119">
+      <c r="J30" s="116">
         <v>2.469E-2</v>
       </c>
-      <c r="M30" s="159"/>
-      <c r="N30" s="162"/>
-      <c r="O30" s="162"/>
+      <c r="K30" s="149"/>
+      <c r="L30" s="152"/>
+      <c r="M30" s="152"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="137"/>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="127"/>
       <c r="B31" s="7">
         <v>4</v>
       </c>
-      <c r="C31" s="138"/>
-      <c r="D31" s="138"/>
-      <c r="E31" s="111">
-        <v>46</v>
-      </c>
-      <c r="F31" s="26">
+      <c r="C31" s="128"/>
+      <c r="D31" s="26">
         <v>40.5</v>
       </c>
-      <c r="G31" s="26">
+      <c r="E31" s="26">
         <f t="shared" si="0"/>
         <v>314.64999999999998</v>
       </c>
-      <c r="H31" s="107">
+      <c r="F31" s="107">
         <v>25</v>
       </c>
-      <c r="I31" s="116">
+      <c r="G31" s="113">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J31" s="27">
+      <c r="H31" s="27">
         <v>8.8000000000000007</v>
       </c>
-      <c r="K31" s="17">
+      <c r="I31" s="17">
         <v>23.8</v>
       </c>
-      <c r="L31" s="119">
+      <c r="J31" s="116">
         <v>6.3339999999999994E-2</v>
       </c>
-      <c r="M31" s="159"/>
-      <c r="N31" s="162"/>
-      <c r="O31" s="162"/>
+      <c r="K31" s="149"/>
+      <c r="L31" s="152"/>
+      <c r="M31" s="152"/>
     </row>
-    <row r="32" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="150"/>
+    <row r="32" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="140"/>
       <c r="B32" s="8">
         <v>5</v>
       </c>
-      <c r="C32" s="145"/>
-      <c r="D32" s="145"/>
-      <c r="E32" s="113">
-        <v>47</v>
-      </c>
-      <c r="F32" s="26">
+      <c r="C32" s="128"/>
+      <c r="D32" s="26">
         <v>38.950000000000003</v>
       </c>
-      <c r="G32" s="103">
+      <c r="E32" s="103">
         <f t="shared" si="0"/>
         <v>313.09999999999997</v>
       </c>
-      <c r="H32" s="108">
+      <c r="F32" s="108">
         <v>25</v>
       </c>
-      <c r="I32" s="118">
+      <c r="G32" s="115">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J32" s="29">
+      <c r="H32" s="29">
         <v>10</v>
       </c>
-      <c r="K32" s="18">
+      <c r="I32" s="18">
         <v>25</v>
       </c>
-      <c r="L32" s="120">
+      <c r="J32" s="117">
         <v>3.2640000000000002E-2</v>
       </c>
-      <c r="M32" s="160"/>
-      <c r="N32" s="163"/>
-      <c r="O32" s="163"/>
+      <c r="K32" s="150"/>
+      <c r="L32" s="153"/>
+      <c r="M32" s="153"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="164">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="154">
         <v>7</v>
       </c>
-      <c r="B33" s="122">
+      <c r="B33" s="119">
         <v>1</v>
       </c>
-      <c r="C33" s="165">
+      <c r="C33" s="128">
         <v>45</v>
       </c>
-      <c r="D33" s="165">
-        <f t="shared" ref="D33" si="21">C33+273.15</f>
-        <v>318.14999999999998</v>
-      </c>
-      <c r="E33" s="123">
-        <v>33</v>
-      </c>
-      <c r="F33" s="26">
+      <c r="D33" s="26">
         <v>45.25</v>
       </c>
-      <c r="G33" s="126">
+      <c r="E33" s="122">
         <f t="shared" si="0"/>
         <v>319.39999999999998</v>
       </c>
-      <c r="H33" s="127">
+      <c r="F33" s="123">
         <v>25</v>
       </c>
-      <c r="I33" s="128">
+      <c r="G33" s="124">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J33" s="124">
+      <c r="H33" s="120">
         <v>6.6</v>
       </c>
-      <c r="K33" s="125">
+      <c r="I33" s="121">
         <v>21.6</v>
       </c>
-      <c r="L33" s="129">
+      <c r="J33" s="125">
         <v>4.1390000000000003E-2</v>
       </c>
-      <c r="M33" s="158">
-        <f t="shared" ref="M33" si="22">AVERAGE(L33:L37)</f>
+      <c r="K33" s="148">
+        <f t="shared" ref="K33" si="16">AVERAGE(J33:J37)</f>
         <v>9.4269999999999993E-2</v>
       </c>
-      <c r="N33" s="161">
-        <f t="shared" ref="N33" si="23">O33/SQRT(5)</f>
+      <c r="L33" s="151">
+        <f t="shared" ref="L33" si="17">M33/SQRT(5)</f>
         <v>3.0525774846840499E-2</v>
       </c>
-      <c r="O33" s="161">
-        <f t="shared" ref="O33" si="24">_xlfn.STDEV.S(L33:L37)</f>
+      <c r="M33" s="151">
+        <f t="shared" ref="M33" si="18">_xlfn.STDEV.S(J33:J37)</f>
         <v>6.8257707623388592E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="137"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="127"/>
       <c r="B34" s="7">
         <v>2</v>
       </c>
-      <c r="C34" s="138"/>
-      <c r="D34" s="138"/>
-      <c r="E34" s="111">
-        <v>34</v>
-      </c>
-      <c r="F34" s="26">
+      <c r="C34" s="128"/>
+      <c r="D34" s="26">
         <v>43.85</v>
       </c>
-      <c r="G34" s="26">
+      <c r="E34" s="26">
         <f t="shared" si="0"/>
         <v>318</v>
       </c>
-      <c r="H34" s="107">
+      <c r="F34" s="107">
         <v>25</v>
       </c>
-      <c r="I34" s="116">
+      <c r="G34" s="113">
         <v>0.3</v>
       </c>
-      <c r="J34" s="27">
+      <c r="H34" s="27">
         <v>16.2</v>
       </c>
-      <c r="K34" s="17">
+      <c r="I34" s="17">
         <v>31.2</v>
       </c>
-      <c r="L34" s="119">
+      <c r="J34" s="116">
         <v>6.9720000000000004E-2</v>
       </c>
-      <c r="M34" s="159"/>
-      <c r="N34" s="162"/>
-      <c r="O34" s="162"/>
+      <c r="K34" s="149"/>
+      <c r="L34" s="152"/>
+      <c r="M34" s="152"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="137"/>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="127"/>
       <c r="B35" s="7">
         <v>3</v>
       </c>
-      <c r="C35" s="138"/>
-      <c r="D35" s="138"/>
-      <c r="E35" s="111">
-        <v>35</v>
-      </c>
-      <c r="F35" s="26">
+      <c r="C35" s="128"/>
+      <c r="D35" s="26">
         <v>44.8</v>
       </c>
-      <c r="G35" s="26">
+      <c r="E35" s="26">
         <f t="shared" si="0"/>
         <v>318.95</v>
       </c>
-      <c r="H35" s="107">
+      <c r="F35" s="107">
         <v>25</v>
       </c>
-      <c r="I35" s="116">
+      <c r="G35" s="113">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J35" s="27">
+      <c r="H35" s="27">
         <v>4.8</v>
       </c>
-      <c r="K35" s="17">
+      <c r="I35" s="17">
         <v>19.8</v>
       </c>
-      <c r="L35" s="119">
+      <c r="J35" s="116">
         <v>0.19417000000000001</v>
       </c>
-      <c r="M35" s="159"/>
-      <c r="N35" s="162"/>
-      <c r="O35" s="162"/>
+      <c r="K35" s="149"/>
+      <c r="L35" s="152"/>
+      <c r="M35" s="152"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="137"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="127"/>
       <c r="B36" s="7">
         <v>4</v>
       </c>
-      <c r="C36" s="138"/>
-      <c r="D36" s="138"/>
-      <c r="E36" s="111">
-        <v>36</v>
-      </c>
-      <c r="F36" s="26">
+      <c r="C36" s="128"/>
+      <c r="D36" s="26">
         <v>44.6</v>
       </c>
-      <c r="G36" s="26">
+      <c r="E36" s="26">
         <f t="shared" si="0"/>
         <v>318.75</v>
       </c>
-      <c r="H36" s="107">
+      <c r="F36" s="107">
         <v>25</v>
       </c>
-      <c r="I36" s="116">
+      <c r="G36" s="113">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J36" s="27">
+      <c r="H36" s="27">
         <v>8</v>
       </c>
-      <c r="K36" s="17">
+      <c r="I36" s="17">
         <v>23</v>
       </c>
-      <c r="L36" s="119">
+      <c r="J36" s="116">
         <v>0.13306000000000001</v>
       </c>
-      <c r="M36" s="159"/>
-      <c r="N36" s="162"/>
-      <c r="O36" s="162"/>
+      <c r="K36" s="149"/>
+      <c r="L36" s="152"/>
+      <c r="M36" s="152"/>
     </row>
-    <row r="37" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="150"/>
+    <row r="37" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="140"/>
       <c r="B37" s="8">
         <v>5</v>
       </c>
-      <c r="C37" s="145"/>
-      <c r="D37" s="145"/>
-      <c r="E37" s="113">
-        <v>37</v>
-      </c>
-      <c r="F37" s="26">
+      <c r="C37" s="128"/>
+      <c r="D37" s="26">
         <v>44.650000000000006</v>
       </c>
-      <c r="G37" s="103">
+      <c r="E37" s="103">
         <f t="shared" si="0"/>
         <v>318.79999999999995</v>
       </c>
-      <c r="H37" s="108">
+      <c r="F37" s="108">
         <v>25</v>
       </c>
-      <c r="I37" s="118">
+      <c r="G37" s="115">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J37" s="29">
+      <c r="H37" s="29">
         <v>12.4</v>
       </c>
-      <c r="K37" s="18">
+      <c r="I37" s="18">
         <v>27.4</v>
       </c>
-      <c r="L37" s="120">
+      <c r="J37" s="117">
         <v>3.3009999999999998E-2</v>
       </c>
-      <c r="M37" s="160"/>
-      <c r="N37" s="163"/>
-      <c r="O37" s="163"/>
+      <c r="K37" s="150"/>
+      <c r="L37" s="153"/>
+      <c r="M37" s="153"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="164">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="154">
         <v>8</v>
       </c>
-      <c r="B38" s="122">
+      <c r="B38" s="119">
         <v>1</v>
       </c>
-      <c r="C38" s="165">
+      <c r="C38" s="128">
         <v>50</v>
       </c>
-      <c r="D38" s="165">
-        <f t="shared" ref="D38" si="25">C38+273.15</f>
-        <v>323.14999999999998</v>
-      </c>
-      <c r="E38" s="123">
-        <v>38</v>
-      </c>
-      <c r="F38" s="26">
+      <c r="D38" s="26">
         <v>49.3</v>
       </c>
-      <c r="G38" s="126">
+      <c r="E38" s="122">
         <f t="shared" si="0"/>
         <v>323.45</v>
       </c>
-      <c r="H38" s="127">
+      <c r="F38" s="123">
         <v>25</v>
       </c>
-      <c r="I38" s="128">
+      <c r="G38" s="124">
         <v>0.31</v>
       </c>
-      <c r="J38" s="124">
+      <c r="H38" s="120">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K38" s="125">
+      <c r="I38" s="121">
         <v>19.600000000000001</v>
       </c>
-      <c r="L38" s="129">
+      <c r="J38" s="125">
         <v>0.17294999999999999</v>
       </c>
-      <c r="M38" s="158">
-        <f t="shared" ref="M38" si="26">AVERAGE(L38:L42)</f>
+      <c r="K38" s="148">
+        <f t="shared" ref="K38" si="19">AVERAGE(J38:J42)</f>
         <v>0.10080799999999998</v>
       </c>
-      <c r="N38" s="161">
-        <f t="shared" ref="N38" si="27">O38/SQRT(5)</f>
+      <c r="L38" s="151">
+        <f t="shared" ref="L38" si="20">M38/SQRT(5)</f>
         <v>2.0893128391890024E-2</v>
       </c>
-      <c r="O38" s="161">
-        <f t="shared" ref="O38" si="28">_xlfn.STDEV.S(L38:L42)</f>
+      <c r="M38" s="151">
+        <f t="shared" ref="M38" si="21">_xlfn.STDEV.S(J38:J42)</f>
         <v>4.6718455346896962E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="137"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="127"/>
       <c r="B39" s="7">
         <v>2</v>
       </c>
-      <c r="C39" s="138"/>
-      <c r="D39" s="138"/>
-      <c r="E39" s="111">
-        <v>39</v>
-      </c>
-      <c r="F39" s="26">
+      <c r="C39" s="128"/>
+      <c r="D39" s="26">
         <v>49.4</v>
       </c>
-      <c r="G39" s="26">
+      <c r="E39" s="26">
         <f t="shared" si="0"/>
         <v>323.54999999999995</v>
       </c>
-      <c r="H39" s="107">
+      <c r="F39" s="107">
         <v>25</v>
       </c>
-      <c r="I39" s="116">
+      <c r="G39" s="113">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J39" s="27">
+      <c r="H39" s="27">
         <v>9.8000000000000007</v>
       </c>
-      <c r="K39" s="17">
+      <c r="I39" s="17">
         <v>24.8</v>
       </c>
-      <c r="L39" s="119">
+      <c r="J39" s="116">
         <v>5.9319999999999998E-2</v>
       </c>
-      <c r="M39" s="159"/>
-      <c r="N39" s="162"/>
-      <c r="O39" s="162"/>
+      <c r="K39" s="149"/>
+      <c r="L39" s="152"/>
+      <c r="M39" s="152"/>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="137"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="127"/>
       <c r="B40" s="7">
         <v>3</v>
       </c>
-      <c r="C40" s="138"/>
-      <c r="D40" s="138"/>
-      <c r="E40" s="111">
-        <v>40</v>
-      </c>
-      <c r="F40" s="26">
+      <c r="C40" s="128"/>
+      <c r="D40" s="26">
         <v>48.55</v>
       </c>
-      <c r="G40" s="26">
+      <c r="E40" s="26">
         <f t="shared" si="0"/>
         <v>322.7</v>
       </c>
-      <c r="H40" s="107">
+      <c r="F40" s="107">
         <v>25</v>
       </c>
-      <c r="I40" s="116">
+      <c r="G40" s="113">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J40" s="27">
+      <c r="H40" s="27">
         <v>11.4</v>
       </c>
-      <c r="K40" s="17">
+      <c r="I40" s="17">
         <v>26.4</v>
       </c>
-      <c r="L40" s="119">
+      <c r="J40" s="116">
         <v>7.1830000000000005E-2</v>
       </c>
-      <c r="M40" s="159"/>
-      <c r="N40" s="162"/>
-      <c r="O40" s="162"/>
+      <c r="K40" s="149"/>
+      <c r="L40" s="152"/>
+      <c r="M40" s="152"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="149"/>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="139"/>
       <c r="B41" s="34">
         <v>4</v>
       </c>
-      <c r="C41" s="144"/>
-      <c r="D41" s="144"/>
-      <c r="E41" s="112">
-        <v>41</v>
-      </c>
-      <c r="F41" s="26">
+      <c r="C41" s="134"/>
+      <c r="D41" s="26">
         <v>49.45</v>
       </c>
-      <c r="G41" s="26">
+      <c r="E41" s="26">
         <f t="shared" si="0"/>
         <v>323.59999999999997</v>
       </c>
-      <c r="H41" s="107">
+      <c r="F41" s="107">
         <v>25</v>
       </c>
-      <c r="I41" s="117">
+      <c r="G41" s="114">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J41" s="27">
+      <c r="H41" s="27">
         <v>5.2</v>
       </c>
-      <c r="K41" s="17">
+      <c r="I41" s="17">
         <v>20.2</v>
       </c>
-      <c r="L41" s="119">
+      <c r="J41" s="116">
         <v>0.12192</v>
       </c>
-      <c r="M41" s="159"/>
-      <c r="N41" s="162"/>
-      <c r="O41" s="162"/>
+      <c r="K41" s="149"/>
+      <c r="L41" s="152"/>
+      <c r="M41" s="152"/>
     </row>
-    <row r="42" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="150"/>
+    <row r="42" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="140"/>
       <c r="B42" s="8">
         <v>5</v>
       </c>
-      <c r="C42" s="145"/>
-      <c r="D42" s="145"/>
-      <c r="E42" s="113">
-        <v>42</v>
-      </c>
-      <c r="F42" s="103">
+      <c r="C42" s="135"/>
+      <c r="D42" s="103">
         <v>49.8</v>
       </c>
-      <c r="G42" s="103">
+      <c r="E42" s="103">
         <f t="shared" si="0"/>
         <v>323.95</v>
       </c>
-      <c r="H42" s="108">
+      <c r="F42" s="108">
         <v>25</v>
       </c>
-      <c r="I42" s="118">
+      <c r="G42" s="115">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J42" s="29">
+      <c r="H42" s="29">
         <v>11.2</v>
       </c>
-      <c r="K42" s="18">
+      <c r="I42" s="18">
         <v>26.2</v>
       </c>
-      <c r="L42" s="120">
+      <c r="J42" s="117">
         <v>7.8020000000000006E-2</v>
       </c>
-      <c r="M42" s="160"/>
-      <c r="N42" s="163"/>
-      <c r="O42" s="163"/>
+      <c r="K42" s="150"/>
+      <c r="L42" s="153"/>
+      <c r="M42" s="153"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="O28:O32"/>
-    <mergeCell ref="O33:O37"/>
-    <mergeCell ref="O38:O42"/>
-    <mergeCell ref="O8:O12"/>
-    <mergeCell ref="O13:O17"/>
-    <mergeCell ref="O18:O22"/>
-    <mergeCell ref="O23:O27"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="D38:D42"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="D28:D32"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="D33:D37"/>
+  <mergeCells count="42">
+    <mergeCell ref="M28:M32"/>
     <mergeCell ref="M33:M37"/>
     <mergeCell ref="M38:M42"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="N8:N12"/>
-    <mergeCell ref="N13:N17"/>
-    <mergeCell ref="N18:N22"/>
-    <mergeCell ref="N23:N27"/>
-    <mergeCell ref="N28:N32"/>
-    <mergeCell ref="N33:N37"/>
-    <mergeCell ref="N38:N42"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="C38:C42"/>
     <mergeCell ref="M8:M12"/>
     <mergeCell ref="M13:M17"/>
     <mergeCell ref="M18:M22"/>
     <mergeCell ref="M23:M27"/>
-    <mergeCell ref="M28:M32"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="K33:K37"/>
+    <mergeCell ref="K38:K42"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="L8:L12"/>
+    <mergeCell ref="L13:L17"/>
+    <mergeCell ref="L18:L22"/>
+    <mergeCell ref="L23:L27"/>
+    <mergeCell ref="L28:L32"/>
+    <mergeCell ref="L33:L37"/>
+    <mergeCell ref="L38:L42"/>
+    <mergeCell ref="K8:K12"/>
+    <mergeCell ref="K13:K17"/>
+    <mergeCell ref="K18:K22"/>
+    <mergeCell ref="K23:K27"/>
+    <mergeCell ref="K28:K32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="M3:M42 O3:O42" formulaRange="1"/>
+    <ignoredError sqref="K3:K42 M3:M42" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6533,7 +6275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0C1EC3-6CE7-1240-A693-968030CFB155}">
   <dimension ref="A1:CC305"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -6624,351 +6366,351 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:81" ht="25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="G1" s="178"/>
-      <c r="H1" s="178"/>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
-      <c r="K1" s="178"/>
-      <c r="L1" s="178"/>
-      <c r="M1" s="178"/>
-      <c r="N1" s="178"/>
-      <c r="O1" s="178"/>
-      <c r="P1" s="178"/>
-      <c r="Q1" s="178"/>
-      <c r="R1" s="178"/>
-      <c r="S1" s="178"/>
-      <c r="T1" s="178"/>
-      <c r="U1" s="178"/>
-      <c r="V1" s="178"/>
-      <c r="W1" s="178"/>
-      <c r="X1" s="178"/>
-      <c r="Y1" s="178"/>
-      <c r="Z1" s="178"/>
-      <c r="AA1" s="178"/>
-      <c r="AB1" s="178"/>
-      <c r="AC1" s="178"/>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
-      <c r="AF1" s="178"/>
-      <c r="AG1" s="178"/>
-      <c r="AH1" s="178"/>
-      <c r="AI1" s="178"/>
-      <c r="AJ1" s="178"/>
-      <c r="AK1" s="178"/>
-      <c r="AL1" s="178"/>
-      <c r="AM1" s="178"/>
-      <c r="AN1" s="178"/>
-      <c r="AO1" s="178"/>
-      <c r="AP1" s="178"/>
-      <c r="AQ1" s="178"/>
-      <c r="AR1" s="178"/>
-      <c r="AS1" s="178"/>
-      <c r="AT1" s="178"/>
-      <c r="AU1" s="178"/>
-      <c r="AV1" s="178"/>
-      <c r="AW1" s="178"/>
-      <c r="AX1" s="178"/>
-      <c r="AY1" s="178"/>
-      <c r="AZ1" s="178"/>
-      <c r="BA1" s="178"/>
-      <c r="BB1" s="178"/>
-      <c r="BC1" s="178"/>
-      <c r="BD1" s="178"/>
-      <c r="BE1" s="178"/>
-      <c r="BF1" s="178"/>
-      <c r="BG1" s="178"/>
-      <c r="BH1" s="178"/>
-      <c r="BI1" s="178"/>
-      <c r="BJ1" s="178"/>
-      <c r="BK1" s="178"/>
-      <c r="BL1" s="178"/>
-      <c r="BM1" s="178"/>
-      <c r="BN1" s="178"/>
-      <c r="BO1" s="178"/>
-      <c r="BP1" s="178"/>
-      <c r="BQ1" s="178"/>
-      <c r="BR1" s="178"/>
-      <c r="BS1" s="178"/>
-      <c r="BT1" s="178"/>
-      <c r="BU1" s="178"/>
-      <c r="BV1" s="178"/>
-      <c r="BW1" s="178"/>
-      <c r="BX1" s="178"/>
-      <c r="BY1" s="178"/>
-      <c r="BZ1" s="178"/>
-      <c r="CA1" s="178"/>
-      <c r="CB1" s="178"/>
-      <c r="CC1" s="179"/>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="L1" s="167"/>
+      <c r="M1" s="167"/>
+      <c r="N1" s="167"/>
+      <c r="O1" s="167"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="167"/>
+      <c r="AB1" s="167"/>
+      <c r="AC1" s="167"/>
+      <c r="AD1" s="167"/>
+      <c r="AE1" s="167"/>
+      <c r="AF1" s="167"/>
+      <c r="AG1" s="167"/>
+      <c r="AH1" s="167"/>
+      <c r="AI1" s="167"/>
+      <c r="AJ1" s="167"/>
+      <c r="AK1" s="167"/>
+      <c r="AL1" s="167"/>
+      <c r="AM1" s="167"/>
+      <c r="AN1" s="167"/>
+      <c r="AO1" s="167"/>
+      <c r="AP1" s="167"/>
+      <c r="AQ1" s="167"/>
+      <c r="AR1" s="167"/>
+      <c r="AS1" s="167"/>
+      <c r="AT1" s="167"/>
+      <c r="AU1" s="167"/>
+      <c r="AV1" s="167"/>
+      <c r="AW1" s="167"/>
+      <c r="AX1" s="167"/>
+      <c r="AY1" s="167"/>
+      <c r="AZ1" s="167"/>
+      <c r="BA1" s="167"/>
+      <c r="BB1" s="167"/>
+      <c r="BC1" s="167"/>
+      <c r="BD1" s="167"/>
+      <c r="BE1" s="167"/>
+      <c r="BF1" s="167"/>
+      <c r="BG1" s="167"/>
+      <c r="BH1" s="167"/>
+      <c r="BI1" s="167"/>
+      <c r="BJ1" s="167"/>
+      <c r="BK1" s="167"/>
+      <c r="BL1" s="167"/>
+      <c r="BM1" s="167"/>
+      <c r="BN1" s="167"/>
+      <c r="BO1" s="167"/>
+      <c r="BP1" s="167"/>
+      <c r="BQ1" s="167"/>
+      <c r="BR1" s="167"/>
+      <c r="BS1" s="167"/>
+      <c r="BT1" s="167"/>
+      <c r="BU1" s="167"/>
+      <c r="BV1" s="167"/>
+      <c r="BW1" s="167"/>
+      <c r="BX1" s="167"/>
+      <c r="BY1" s="167"/>
+      <c r="BZ1" s="167"/>
+      <c r="CA1" s="167"/>
+      <c r="CB1" s="167"/>
+      <c r="CC1" s="168"/>
     </row>
     <row r="2" spans="1:81" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="170"/>
-      <c r="B2" s="180" t="s">
+      <c r="A2" s="159"/>
+      <c r="B2" s="169" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="181"/>
-      <c r="G2" s="181"/>
-      <c r="H2" s="181"/>
-      <c r="I2" s="181"/>
-      <c r="J2" s="181"/>
-      <c r="K2" s="181"/>
-      <c r="L2" s="181" t="s">
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="170"/>
+      <c r="I2" s="170"/>
+      <c r="J2" s="170"/>
+      <c r="K2" s="170"/>
+      <c r="L2" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="181"/>
-      <c r="N2" s="181"/>
-      <c r="O2" s="181"/>
-      <c r="P2" s="181"/>
-      <c r="Q2" s="181"/>
-      <c r="R2" s="181"/>
-      <c r="S2" s="181"/>
-      <c r="T2" s="181"/>
-      <c r="U2" s="181"/>
-      <c r="V2" s="181" t="s">
+      <c r="M2" s="170"/>
+      <c r="N2" s="170"/>
+      <c r="O2" s="170"/>
+      <c r="P2" s="170"/>
+      <c r="Q2" s="170"/>
+      <c r="R2" s="170"/>
+      <c r="S2" s="170"/>
+      <c r="T2" s="170"/>
+      <c r="U2" s="170"/>
+      <c r="V2" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="181"/>
-      <c r="X2" s="181"/>
-      <c r="Y2" s="181"/>
-      <c r="Z2" s="181"/>
-      <c r="AA2" s="181"/>
-      <c r="AB2" s="181"/>
-      <c r="AC2" s="181"/>
-      <c r="AD2" s="181"/>
-      <c r="AE2" s="181"/>
-      <c r="AF2" s="181" t="s">
+      <c r="W2" s="170"/>
+      <c r="X2" s="170"/>
+      <c r="Y2" s="170"/>
+      <c r="Z2" s="170"/>
+      <c r="AA2" s="170"/>
+      <c r="AB2" s="170"/>
+      <c r="AC2" s="170"/>
+      <c r="AD2" s="170"/>
+      <c r="AE2" s="170"/>
+      <c r="AF2" s="170" t="s">
         <v>40</v>
       </c>
-      <c r="AG2" s="181"/>
-      <c r="AH2" s="181"/>
-      <c r="AI2" s="181"/>
-      <c r="AJ2" s="181"/>
-      <c r="AK2" s="181"/>
-      <c r="AL2" s="181"/>
-      <c r="AM2" s="181"/>
-      <c r="AN2" s="181"/>
-      <c r="AO2" s="181"/>
-      <c r="AP2" s="181" t="s">
+      <c r="AG2" s="170"/>
+      <c r="AH2" s="170"/>
+      <c r="AI2" s="170"/>
+      <c r="AJ2" s="170"/>
+      <c r="AK2" s="170"/>
+      <c r="AL2" s="170"/>
+      <c r="AM2" s="170"/>
+      <c r="AN2" s="170"/>
+      <c r="AO2" s="170"/>
+      <c r="AP2" s="170" t="s">
         <v>41</v>
       </c>
-      <c r="AQ2" s="181"/>
-      <c r="AR2" s="181"/>
-      <c r="AS2" s="181"/>
-      <c r="AT2" s="181"/>
-      <c r="AU2" s="181"/>
-      <c r="AV2" s="181"/>
-      <c r="AW2" s="181"/>
-      <c r="AX2" s="181"/>
-      <c r="AY2" s="181"/>
-      <c r="AZ2" s="181" t="s">
+      <c r="AQ2" s="170"/>
+      <c r="AR2" s="170"/>
+      <c r="AS2" s="170"/>
+      <c r="AT2" s="170"/>
+      <c r="AU2" s="170"/>
+      <c r="AV2" s="170"/>
+      <c r="AW2" s="170"/>
+      <c r="AX2" s="170"/>
+      <c r="AY2" s="170"/>
+      <c r="AZ2" s="170" t="s">
         <v>42</v>
       </c>
-      <c r="BA2" s="181"/>
-      <c r="BB2" s="181"/>
-      <c r="BC2" s="181"/>
-      <c r="BD2" s="181"/>
-      <c r="BE2" s="181"/>
-      <c r="BF2" s="181"/>
-      <c r="BG2" s="181"/>
-      <c r="BH2" s="181"/>
-      <c r="BI2" s="181"/>
-      <c r="BJ2" s="181" t="s">
+      <c r="BA2" s="170"/>
+      <c r="BB2" s="170"/>
+      <c r="BC2" s="170"/>
+      <c r="BD2" s="170"/>
+      <c r="BE2" s="170"/>
+      <c r="BF2" s="170"/>
+      <c r="BG2" s="170"/>
+      <c r="BH2" s="170"/>
+      <c r="BI2" s="170"/>
+      <c r="BJ2" s="170" t="s">
         <v>43</v>
       </c>
-      <c r="BK2" s="181"/>
-      <c r="BL2" s="181"/>
-      <c r="BM2" s="181"/>
-      <c r="BN2" s="181"/>
-      <c r="BO2" s="181"/>
-      <c r="BP2" s="181"/>
-      <c r="BQ2" s="181"/>
-      <c r="BR2" s="181"/>
-      <c r="BS2" s="181"/>
-      <c r="BT2" s="181" t="s">
+      <c r="BK2" s="170"/>
+      <c r="BL2" s="170"/>
+      <c r="BM2" s="170"/>
+      <c r="BN2" s="170"/>
+      <c r="BO2" s="170"/>
+      <c r="BP2" s="170"/>
+      <c r="BQ2" s="170"/>
+      <c r="BR2" s="170"/>
+      <c r="BS2" s="170"/>
+      <c r="BT2" s="170" t="s">
         <v>44</v>
       </c>
-      <c r="BU2" s="181"/>
-      <c r="BV2" s="181"/>
-      <c r="BW2" s="181"/>
-      <c r="BX2" s="181"/>
-      <c r="BY2" s="181"/>
-      <c r="BZ2" s="181"/>
-      <c r="CA2" s="181"/>
-      <c r="CB2" s="181"/>
-      <c r="CC2" s="182"/>
+      <c r="BU2" s="170"/>
+      <c r="BV2" s="170"/>
+      <c r="BW2" s="170"/>
+      <c r="BX2" s="170"/>
+      <c r="BY2" s="170"/>
+      <c r="BZ2" s="170"/>
+      <c r="CA2" s="170"/>
+      <c r="CB2" s="170"/>
+      <c r="CC2" s="171"/>
     </row>
     <row r="3" spans="1:81" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="171"/>
-      <c r="B3" s="168" t="s">
+      <c r="A3" s="160"/>
+      <c r="B3" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="169"/>
-      <c r="D3" s="172" t="s">
+      <c r="C3" s="158"/>
+      <c r="D3" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="173"/>
-      <c r="F3" s="172" t="s">
+      <c r="E3" s="162"/>
+      <c r="F3" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="173"/>
-      <c r="H3" s="172" t="s">
+      <c r="G3" s="162"/>
+      <c r="H3" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="173"/>
-      <c r="J3" s="174" t="s">
+      <c r="I3" s="162"/>
+      <c r="J3" s="163" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="175"/>
-      <c r="L3" s="172" t="s">
+      <c r="K3" s="164"/>
+      <c r="L3" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="173"/>
-      <c r="N3" s="172" t="s">
+      <c r="M3" s="162"/>
+      <c r="N3" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="173"/>
-      <c r="P3" s="172" t="s">
+      <c r="O3" s="162"/>
+      <c r="P3" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="173"/>
-      <c r="R3" s="172" t="s">
+      <c r="Q3" s="162"/>
+      <c r="R3" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="173"/>
-      <c r="T3" s="172" t="s">
+      <c r="S3" s="162"/>
+      <c r="T3" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="173"/>
-      <c r="V3" s="172" t="s">
+      <c r="U3" s="162"/>
+      <c r="V3" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="W3" s="173"/>
-      <c r="X3" s="172" t="s">
+      <c r="W3" s="162"/>
+      <c r="X3" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="173"/>
-      <c r="Z3" s="172" t="s">
+      <c r="Y3" s="162"/>
+      <c r="Z3" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="AA3" s="173"/>
-      <c r="AB3" s="172" t="s">
+      <c r="AA3" s="162"/>
+      <c r="AB3" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="173"/>
-      <c r="AD3" s="172" t="s">
+      <c r="AC3" s="162"/>
+      <c r="AD3" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="AE3" s="173"/>
-      <c r="AF3" s="172" t="s">
+      <c r="AE3" s="162"/>
+      <c r="AF3" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="AG3" s="173"/>
-      <c r="AH3" s="172" t="s">
+      <c r="AG3" s="162"/>
+      <c r="AH3" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="AI3" s="173"/>
-      <c r="AJ3" s="172" t="s">
+      <c r="AI3" s="162"/>
+      <c r="AJ3" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="AK3" s="173"/>
-      <c r="AL3" s="172" t="s">
+      <c r="AK3" s="162"/>
+      <c r="AL3" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="AM3" s="173"/>
-      <c r="AN3" s="172" t="s">
+      <c r="AM3" s="162"/>
+      <c r="AN3" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="AO3" s="173"/>
-      <c r="AP3" s="172" t="s">
+      <c r="AO3" s="162"/>
+      <c r="AP3" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="173"/>
-      <c r="AR3" s="172" t="s">
+      <c r="AQ3" s="162"/>
+      <c r="AR3" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="AS3" s="173"/>
-      <c r="AT3" s="172" t="s">
+      <c r="AS3" s="162"/>
+      <c r="AT3" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="AU3" s="173"/>
-      <c r="AV3" s="172" t="s">
+      <c r="AU3" s="162"/>
+      <c r="AV3" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="AW3" s="173"/>
-      <c r="AX3" s="172" t="s">
+      <c r="AW3" s="162"/>
+      <c r="AX3" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="AY3" s="173"/>
-      <c r="AZ3" s="172" t="s">
+      <c r="AY3" s="162"/>
+      <c r="AZ3" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="BA3" s="173"/>
-      <c r="BB3" s="172" t="s">
+      <c r="BA3" s="162"/>
+      <c r="BB3" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="BC3" s="173"/>
-      <c r="BD3" s="172" t="s">
+      <c r="BC3" s="162"/>
+      <c r="BD3" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="BE3" s="173"/>
-      <c r="BF3" s="172" t="s">
+      <c r="BE3" s="162"/>
+      <c r="BF3" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="BG3" s="173"/>
-      <c r="BH3" s="172" t="s">
+      <c r="BG3" s="162"/>
+      <c r="BH3" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="BI3" s="173"/>
-      <c r="BJ3" s="172" t="s">
+      <c r="BI3" s="162"/>
+      <c r="BJ3" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="BK3" s="173"/>
-      <c r="BL3" s="172" t="s">
+      <c r="BK3" s="162"/>
+      <c r="BL3" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="BM3" s="173"/>
-      <c r="BN3" s="172" t="s">
+      <c r="BM3" s="162"/>
+      <c r="BN3" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="BO3" s="173"/>
-      <c r="BP3" s="172" t="s">
+      <c r="BO3" s="162"/>
+      <c r="BP3" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="BQ3" s="173"/>
-      <c r="BR3" s="176" t="s">
+      <c r="BQ3" s="162"/>
+      <c r="BR3" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="BS3" s="169"/>
-      <c r="BT3" s="172" t="s">
+      <c r="BS3" s="158"/>
+      <c r="BT3" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="BU3" s="173"/>
-      <c r="BV3" s="172" t="s">
+      <c r="BU3" s="162"/>
+      <c r="BV3" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="BW3" s="173"/>
-      <c r="BX3" s="172" t="s">
+      <c r="BW3" s="162"/>
+      <c r="BX3" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="BY3" s="173"/>
-      <c r="BZ3" s="172" t="s">
+      <c r="BY3" s="162"/>
+      <c r="BZ3" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="CA3" s="173"/>
-      <c r="CB3" s="172" t="s">
+      <c r="CA3" s="162"/>
+      <c r="CB3" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="CC3" s="173"/>
+      <c r="CC3" s="162"/>
     </row>
     <row r="4" spans="1:81" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">

</xml_diff>

<commit_message>
last commit before sleep
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wrca-my.sharepoint.com/personal/huj26_mywrca_ca/Documents/12/Chemistry HL/Chemistry IA/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1781" documentId="8_{ED69E5BD-9A97-5849-9651-1A764BC4410F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05FDAB0B-4D7F-B64C-9457-289D613BAFB2}"/>
+  <xr:revisionPtr revIDLastSave="1806" documentId="8_{ED69E5BD-9A97-5849-9651-1A764BC4410F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C9DB826-A043-E644-8AEF-10A12F5E9C9D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{3196E468-6A35-EA40-9409-42F714E37880}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{3196E468-6A35-EA40-9409-42F714E37880}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Processed Data" sheetId="4" r:id="rId2"/>
-    <sheet name="Raw Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Example Calculations" sheetId="5" r:id="rId3"/>
+    <sheet name="Raw Data" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="58">
   <si>
     <t>Target (°C)</t>
   </si>
@@ -246,6 +247,12 @@
   </si>
   <si>
     <t>Initial Rate SD (kPa/s)</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>Temp</t>
   </si>
 </sst>
 </file>
@@ -2234,6 +2241,990 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Pressure vs. Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.43546027742749055"/>
+          <c:y val="1.4342629482071713E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Example Calculations'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pressure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.2282968096831534E-3"/>
+                  <c:y val="6.4249960786774168E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t>y = 0.0059x + 101.35</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                      <a:t>R² = 0.4056</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2000"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Example Calculations'!$A$2:$A$77</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>26.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>31.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>32.6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>33.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>33.6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>33.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>34.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>34.4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>34.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>34.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>35.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>35.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>35.6</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>36.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>36.4</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>36.6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>36.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>37.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>37.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>37.6</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>37.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>38.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>38.4</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>38.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>39.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>39.4</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>39.6</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>39.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>40.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>40.4</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>40.6</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>40.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>41.2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>41.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>41.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Example Calculations'!$C$2:$C$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>101.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>101.48</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>101.48</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>101.48</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>101.48</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>101.48</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>101.67</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>101.54</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>101.67</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>101.67</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>101.61</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>101.61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C413-5445-AAAD-2F55B247FD03}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1646097456"/>
+        <c:axId val="1645592272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1646097456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="41.6"/>
+          <c:min val="26.6"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time / s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1645592272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1645592272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pressure / kPa</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1646097456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2274,7 +3265,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2831,6 +4378,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCB69AC3-41AE-493B-C068-C4DF147D5DB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3150,8 +4738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFD131A-068C-8045-AE76-58186661ABFD}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6272,11 +7860,874 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5EB00A2-2750-2645-87AC-0B0679AEC0D0}">
+  <dimension ref="A1:C77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="88">
+        <v>26.6</v>
+      </c>
+      <c r="B2" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C2" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="88">
+        <v>26.8</v>
+      </c>
+      <c r="B3" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C3" s="58">
+        <v>101.48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="88">
+        <v>27</v>
+      </c>
+      <c r="B4" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C4" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="88">
+        <v>27.2</v>
+      </c>
+      <c r="B5" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C5" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="88">
+        <v>27.4</v>
+      </c>
+      <c r="B6" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C6" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="88">
+        <v>27.6</v>
+      </c>
+      <c r="B7" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C7" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="88">
+        <v>27.8</v>
+      </c>
+      <c r="B8" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C8" s="58">
+        <v>101.48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="88">
+        <v>28</v>
+      </c>
+      <c r="B9" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C9" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="88">
+        <v>28.2</v>
+      </c>
+      <c r="B10" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C10" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="88">
+        <v>28.4</v>
+      </c>
+      <c r="B11" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C11" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="88">
+        <v>28.6</v>
+      </c>
+      <c r="B12" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C12" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="88">
+        <v>28.8</v>
+      </c>
+      <c r="B13" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C13" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="88">
+        <v>29</v>
+      </c>
+      <c r="B14" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C14" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="88">
+        <v>29.2</v>
+      </c>
+      <c r="B15" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C15" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="88">
+        <v>29.4</v>
+      </c>
+      <c r="B16" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C16" s="58">
+        <v>101.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="88">
+        <v>29.6</v>
+      </c>
+      <c r="B17" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C17" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="88">
+        <v>29.8</v>
+      </c>
+      <c r="B18" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C18" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="88">
+        <v>30</v>
+      </c>
+      <c r="B19" s="85">
+        <v>14.6</v>
+      </c>
+      <c r="C19" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="88">
+        <v>30.2</v>
+      </c>
+      <c r="B20" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C20" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="88">
+        <v>30.4</v>
+      </c>
+      <c r="B21" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C21" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="88">
+        <v>30.6</v>
+      </c>
+      <c r="B22" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C22" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="88">
+        <v>30.8</v>
+      </c>
+      <c r="B23" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C23" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="88">
+        <v>31</v>
+      </c>
+      <c r="B24" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C24" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="88">
+        <v>31.2</v>
+      </c>
+      <c r="B25" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C25" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="88">
+        <v>31.4</v>
+      </c>
+      <c r="B26" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C26" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="88">
+        <v>31.6</v>
+      </c>
+      <c r="B27" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C27" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="88">
+        <v>31.8</v>
+      </c>
+      <c r="B28" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C28" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="88">
+        <v>32</v>
+      </c>
+      <c r="B29" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C29" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="88">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="B30" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C30" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="88">
+        <v>32.4</v>
+      </c>
+      <c r="B31" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C31" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="88">
+        <v>32.6</v>
+      </c>
+      <c r="B32" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C32" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="88">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="B33" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C33" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="88">
+        <v>33</v>
+      </c>
+      <c r="B34" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C34" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="88">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="B35" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C35" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="88">
+        <v>33.4</v>
+      </c>
+      <c r="B36" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C36" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="88">
+        <v>33.6</v>
+      </c>
+      <c r="B37" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C37" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="88">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="B38" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C38" s="58">
+        <v>101.48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="88">
+        <v>34</v>
+      </c>
+      <c r="B39" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C39" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="88">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="B40" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C40" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="88">
+        <v>34.4</v>
+      </c>
+      <c r="B41" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C41" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="88">
+        <v>34.6</v>
+      </c>
+      <c r="B42" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C42" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="88">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="B43" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C43" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="88">
+        <v>35</v>
+      </c>
+      <c r="B44" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C44" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="88">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="B45" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C45" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="88">
+        <v>35.4</v>
+      </c>
+      <c r="B46" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C46" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="88">
+        <v>35.6</v>
+      </c>
+      <c r="B47" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C47" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="88">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="B48" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C48" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="88">
+        <v>36</v>
+      </c>
+      <c r="B49" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C49" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="88">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B50" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C50" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="88">
+        <v>36.4</v>
+      </c>
+      <c r="B51" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C51" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="88">
+        <v>36.6</v>
+      </c>
+      <c r="B52" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C52" s="58">
+        <v>101.48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="88">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="B53" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C53" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="88">
+        <v>37</v>
+      </c>
+      <c r="B54" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C54" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="88">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="B55" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C55" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="88">
+        <v>37.4</v>
+      </c>
+      <c r="B56" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C56" s="58">
+        <v>101.48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="88">
+        <v>37.6</v>
+      </c>
+      <c r="B57" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C57" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="88">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="B58" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C58" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="88">
+        <v>38</v>
+      </c>
+      <c r="B59" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C59" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="88">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="B60" s="85">
+        <v>14.7</v>
+      </c>
+      <c r="C60" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="88">
+        <v>38.4</v>
+      </c>
+      <c r="B61" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C61" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="88">
+        <v>38.6</v>
+      </c>
+      <c r="B62" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C62" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="88">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="B63" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C63" s="58">
+        <v>101.67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="88">
+        <v>39</v>
+      </c>
+      <c r="B64" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C64" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="88">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="B65" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C65" s="58">
+        <v>101.54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="88">
+        <v>39.4</v>
+      </c>
+      <c r="B66" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C66" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="88">
+        <v>39.6</v>
+      </c>
+      <c r="B67" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C67" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="88">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="B68" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C68" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="88">
+        <v>40</v>
+      </c>
+      <c r="B69" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C69" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="88">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="B70" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C70" s="58">
+        <v>101.67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="88">
+        <v>40.4</v>
+      </c>
+      <c r="B71" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C71" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="88">
+        <v>40.6</v>
+      </c>
+      <c r="B72" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C72" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="88">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="B73" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C73" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="88">
+        <v>41</v>
+      </c>
+      <c r="B74" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C74" s="58">
+        <v>101.67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="88">
+        <v>41.2</v>
+      </c>
+      <c r="B75" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C75" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="88">
+        <v>41.4</v>
+      </c>
+      <c r="B76" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C76" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="88">
+        <v>41.6</v>
+      </c>
+      <c r="B77" s="85">
+        <v>14.8</v>
+      </c>
+      <c r="C77" s="58">
+        <v>101.61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0C1EC3-6CE7-1240-A693-968030CFB155}">
   <dimension ref="A1:CC305"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138:C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>